<commit_message>
Added tests for tropical location
</commit_message>
<xml_diff>
--- a/Tests/Validation/Weather/Observed.xlsx
+++ b/Tests/Validation/Weather/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E8032-3576-43E3-BFBD-D4E0E7F6E184}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F16C38-A566-40A1-AD27-004DBA9CA254}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="5">
   <si>
     <t>SimulationName</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Clock.Today</t>
+  </si>
+  <si>
+    <t>DarwinRadiation</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -146,9 +148,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE028B48-E928-4E9E-80FD-208C4FFEA9B6}">
   <dimension ref="A1:AC364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183:C363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5795,9 +5798,9 @@
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
       <c r="X150" s="1"/>
-      <c r="Y150" s="11"/>
-      <c r="Z150" s="11"/>
-      <c r="AA150" s="11"/>
+      <c r="Y150" s="10"/>
+      <c r="Z150" s="10"/>
+      <c r="AA150" s="10"/>
     </row>
     <row r="151" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A151" s="5" t="s">
@@ -5830,9 +5833,9 @@
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
       <c r="X151" s="1"/>
-      <c r="Y151" s="11"/>
-      <c r="Z151" s="11"/>
-      <c r="AA151" s="11"/>
+      <c r="Y151" s="10"/>
+      <c r="Z151" s="10"/>
+      <c r="AA151" s="10"/>
     </row>
     <row r="152" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A152" s="5" t="s">
@@ -5865,9 +5868,9 @@
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
       <c r="X152" s="1"/>
-      <c r="Y152" s="11"/>
-      <c r="Z152" s="11"/>
-      <c r="AA152" s="11"/>
+      <c r="Y152" s="10"/>
+      <c r="Z152" s="10"/>
+      <c r="AA152" s="10"/>
     </row>
     <row r="153" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A153" s="5" t="s">
@@ -5900,9 +5903,9 @@
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
       <c r="X153" s="1"/>
-      <c r="Y153" s="11"/>
-      <c r="Z153" s="11"/>
-      <c r="AA153" s="11"/>
+      <c r="Y153" s="10"/>
+      <c r="Z153" s="10"/>
+      <c r="AA153" s="10"/>
     </row>
     <row r="154" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A154" s="5" t="s">
@@ -5935,9 +5938,9 @@
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
       <c r="X154" s="1"/>
-      <c r="Y154" s="11"/>
-      <c r="Z154" s="11"/>
-      <c r="AA154" s="11"/>
+      <c r="Y154" s="10"/>
+      <c r="Z154" s="10"/>
+      <c r="AA154" s="10"/>
     </row>
     <row r="155" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A155" s="5" t="s">
@@ -5970,8 +5973,8 @@
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
-      <c r="Y155" s="11"/>
-      <c r="Z155" s="11"/>
+      <c r="Y155" s="10"/>
+      <c r="Z155" s="10"/>
       <c r="AA155" s="1"/>
     </row>
     <row r="156" spans="1:27" x14ac:dyDescent="0.5">
@@ -6334,10 +6337,10 @@
       <c r="C166">
         <v>0.51018746268026705</v>
       </c>
-      <c r="D166" s="12"/>
-      <c r="E166" s="12"/>
-      <c r="F166" s="13"/>
-      <c r="G166" s="13"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="12"/>
+      <c r="G166" s="12"/>
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
       <c r="J166" s="1"/>
@@ -6370,9 +6373,9 @@
         <v>0.70592686695619467</v>
       </c>
       <c r="D167" s="6"/>
-      <c r="E167" s="12"/>
-      <c r="F167" s="13"/>
-      <c r="G167" s="13"/>
+      <c r="E167" s="11"/>
+      <c r="F167" s="12"/>
+      <c r="G167" s="12"/>
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
       <c r="J167" s="1"/>
@@ -6404,10 +6407,10 @@
       <c r="C168">
         <v>0.82774716448828856</v>
       </c>
-      <c r="D168" s="12"/>
-      <c r="E168" s="12"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
+      <c r="D168" s="11"/>
+      <c r="E168" s="11"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
       <c r="J168" s="1"/>
@@ -6439,10 +6442,10 @@
       <c r="C169">
         <v>0.99769625648344373</v>
       </c>
-      <c r="D169" s="12"/>
-      <c r="E169" s="12"/>
-      <c r="F169" s="13"/>
-      <c r="G169" s="13"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="12"/>
+      <c r="G169" s="12"/>
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
       <c r="J169" s="1"/>
@@ -6474,10 +6477,10 @@
       <c r="C170">
         <v>0.18266864908638383</v>
       </c>
-      <c r="D170" s="12"/>
-      <c r="E170" s="12"/>
-      <c r="F170" s="13"/>
-      <c r="G170" s="13"/>
+      <c r="D170" s="11"/>
+      <c r="E170" s="11"/>
+      <c r="F170" s="12"/>
+      <c r="G170" s="12"/>
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
       <c r="J170" s="1"/>
@@ -6509,10 +6512,10 @@
       <c r="C171">
         <v>0.12829504770615469</v>
       </c>
-      <c r="D171" s="12"/>
-      <c r="E171" s="12"/>
-      <c r="F171" s="13"/>
-      <c r="G171" s="13"/>
+      <c r="D171" s="11"/>
+      <c r="E171" s="11"/>
+      <c r="F171" s="12"/>
+      <c r="G171" s="12"/>
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
       <c r="J171" s="1"/>
@@ -6544,10 +6547,10 @@
       <c r="C172">
         <v>0.27573032010066778</v>
       </c>
-      <c r="D172" s="12"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="13"/>
-      <c r="G172" s="13"/>
+      <c r="D172" s="11"/>
+      <c r="E172" s="11"/>
+      <c r="F172" s="12"/>
+      <c r="G172" s="12"/>
       <c r="H172" s="1"/>
       <c r="I172" s="8"/>
       <c r="J172" s="1"/>
@@ -6580,9 +6583,9 @@
         <v>0.28120042331806799</v>
       </c>
       <c r="D173" s="6"/>
-      <c r="E173" s="12"/>
-      <c r="F173" s="13"/>
-      <c r="G173" s="13"/>
+      <c r="E173" s="11"/>
+      <c r="F173" s="12"/>
+      <c r="G173" s="12"/>
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="1"/>
@@ -6631,12 +6634,12 @@
       <c r="R174" s="1"/>
       <c r="S174" s="1"/>
       <c r="T174" s="1"/>
-      <c r="U174" s="14"/>
+      <c r="U174" s="13"/>
       <c r="V174" s="1"/>
       <c r="W174" s="1"/>
       <c r="X174" s="1"/>
       <c r="Y174" s="1"/>
-      <c r="Z174" s="14"/>
+      <c r="Z174" s="13"/>
       <c r="AA174" s="1"/>
     </row>
     <row r="175" spans="1:27" x14ac:dyDescent="0.5">
@@ -6666,12 +6669,12 @@
       <c r="R175" s="1"/>
       <c r="S175" s="1"/>
       <c r="T175" s="1"/>
-      <c r="U175" s="14"/>
+      <c r="U175" s="13"/>
       <c r="V175" s="1"/>
       <c r="W175" s="1"/>
       <c r="X175" s="1"/>
       <c r="Y175" s="1"/>
-      <c r="Z175" s="15"/>
+      <c r="Z175" s="14"/>
       <c r="AA175" s="1"/>
     </row>
     <row r="176" spans="1:27" x14ac:dyDescent="0.5">
@@ -6701,12 +6704,12 @@
       <c r="R176" s="1"/>
       <c r="S176" s="1"/>
       <c r="T176" s="1"/>
-      <c r="U176" s="14"/>
+      <c r="U176" s="13"/>
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
       <c r="X176" s="1"/>
       <c r="Y176" s="1"/>
-      <c r="Z176" s="14"/>
+      <c r="Z176" s="13"/>
       <c r="AA176" s="1"/>
     </row>
     <row r="177" spans="1:27" x14ac:dyDescent="0.5">
@@ -6736,12 +6739,12 @@
       <c r="R177" s="1"/>
       <c r="S177" s="1"/>
       <c r="T177" s="1"/>
-      <c r="U177" s="16"/>
+      <c r="U177" s="15"/>
       <c r="V177" s="1"/>
       <c r="W177" s="1"/>
       <c r="X177" s="1"/>
       <c r="Y177" s="1"/>
-      <c r="Z177" s="14"/>
+      <c r="Z177" s="13"/>
       <c r="AA177" s="1"/>
     </row>
     <row r="178" spans="1:27" x14ac:dyDescent="0.5">
@@ -6754,10 +6757,10 @@
       <c r="C178">
         <v>0.13916411340672447</v>
       </c>
-      <c r="D178" s="12"/>
+      <c r="D178" s="11"/>
       <c r="E178" s="6"/>
       <c r="F178" s="2"/>
-      <c r="G178" s="13"/>
+      <c r="G178" s="12"/>
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
       <c r="J178" s="1"/>
@@ -6789,10 +6792,10 @@
       <c r="C179">
         <v>0.46197302425561726</v>
       </c>
-      <c r="D179" s="12"/>
+      <c r="D179" s="11"/>
       <c r="E179" s="6"/>
       <c r="F179" s="2"/>
-      <c r="G179" s="13"/>
+      <c r="G179" s="12"/>
       <c r="H179" s="1"/>
       <c r="I179" s="8"/>
       <c r="J179" s="1"/>
@@ -6824,10 +6827,10 @@
       <c r="C180">
         <v>0.61234977835978577</v>
       </c>
-      <c r="D180" s="12"/>
+      <c r="D180" s="11"/>
       <c r="E180" s="6"/>
       <c r="F180" s="2"/>
-      <c r="G180" s="13"/>
+      <c r="G180" s="12"/>
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
       <c r="J180" s="1"/>
@@ -6862,7 +6865,7 @@
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
       <c r="F181" s="2"/>
-      <c r="G181" s="13"/>
+      <c r="G181" s="12"/>
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
       <c r="J181" s="1"/>
@@ -6897,7 +6900,7 @@
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
       <c r="F182" s="2"/>
-      <c r="G182" s="13"/>
+      <c r="G182" s="12"/>
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
       <c r="J182" s="1"/>
@@ -6920,13 +6923,19 @@
       <c r="AA182" s="1"/>
     </row>
     <row r="183" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A183" s="5"/>
-      <c r="B183" s="10"/>
-      <c r="C183" s="6"/>
+      <c r="A183" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B183" s="20">
+        <v>43831</v>
+      </c>
+      <c r="C183" s="7">
+        <v>0.57499689334108006</v>
+      </c>
       <c r="D183" s="1"/>
       <c r="E183" s="6"/>
       <c r="F183" s="2"/>
-      <c r="G183" s="13"/>
+      <c r="G183" s="12"/>
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
@@ -6949,13 +6958,19 @@
       <c r="AA183" s="1"/>
     </row>
     <row r="184" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A184" s="5"/>
-      <c r="B184" s="10"/>
-      <c r="C184" s="6"/>
+      <c r="A184" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184" s="20">
+        <v>43832</v>
+      </c>
+      <c r="C184" s="7">
+        <v>0.52876915616916498</v>
+      </c>
       <c r="D184" s="1"/>
       <c r="E184" s="6"/>
       <c r="F184" s="2"/>
-      <c r="G184" s="13"/>
+      <c r="G184" s="12"/>
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
@@ -6978,13 +6993,19 @@
       <c r="AA184" s="1"/>
     </row>
     <row r="185" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A185" s="5"/>
-      <c r="B185" s="10"/>
-      <c r="C185" s="6"/>
+      <c r="A185" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185" s="20">
+        <v>43833</v>
+      </c>
+      <c r="C185" s="7">
+        <v>0.58785663506769537</v>
+      </c>
       <c r="D185" s="1"/>
       <c r="E185" s="6"/>
       <c r="F185" s="2"/>
-      <c r="G185" s="13"/>
+      <c r="G185" s="12"/>
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
       <c r="J185" s="1"/>
@@ -7007,13 +7028,19 @@
       <c r="AA185" s="1"/>
     </row>
     <row r="186" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A186" s="5"/>
-      <c r="B186" s="10"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="12"/>
+      <c r="A186" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186" s="20">
+        <v>43834</v>
+      </c>
+      <c r="C186" s="7">
+        <v>0.34112371323080948</v>
+      </c>
+      <c r="D186" s="11"/>
       <c r="E186" s="6"/>
       <c r="F186" s="2"/>
-      <c r="G186" s="13"/>
+      <c r="G186" s="12"/>
       <c r="H186" s="1"/>
       <c r="I186" s="8"/>
       <c r="J186" s="1"/>
@@ -7036,13 +7063,19 @@
       <c r="AA186" s="1"/>
     </row>
     <row r="187" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A187" s="5"/>
-      <c r="B187" s="10"/>
-      <c r="C187" s="6"/>
-      <c r="D187" s="12"/>
+      <c r="A187" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" s="20">
+        <v>43835</v>
+      </c>
+      <c r="C187" s="7">
+        <v>0.8637071967772354</v>
+      </c>
+      <c r="D187" s="11"/>
       <c r="E187" s="6"/>
       <c r="F187" s="2"/>
-      <c r="G187" s="13"/>
+      <c r="G187" s="12"/>
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
       <c r="J187" s="1"/>
@@ -7065,13 +7098,19 @@
       <c r="AA187" s="1"/>
     </row>
     <row r="188" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A188" s="5"/>
-      <c r="B188" s="10"/>
-      <c r="C188" s="6"/>
-      <c r="D188" s="12"/>
+      <c r="A188" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188" s="20">
+        <v>43836</v>
+      </c>
+      <c r="C188" s="7">
+        <v>0.68444827362433669</v>
+      </c>
+      <c r="D188" s="11"/>
       <c r="E188" s="6"/>
       <c r="F188" s="2"/>
-      <c r="G188" s="13"/>
+      <c r="G188" s="12"/>
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
       <c r="J188" s="1"/>
@@ -7094,13 +7133,19 @@
       <c r="AA188" s="1"/>
     </row>
     <row r="189" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A189" s="5"/>
-      <c r="B189" s="10"/>
-      <c r="C189" s="6"/>
+      <c r="A189" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" s="20">
+        <v>43837</v>
+      </c>
+      <c r="C189" s="7">
+        <v>0.83044967619754007</v>
+      </c>
       <c r="D189" s="6"/>
       <c r="E189" s="6"/>
       <c r="F189" s="2"/>
-      <c r="G189" s="13"/>
+      <c r="G189" s="12"/>
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
       <c r="J189" s="1"/>
@@ -7123,13 +7168,19 @@
       <c r="AA189" s="1"/>
     </row>
     <row r="190" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A190" s="5"/>
-      <c r="B190" s="10"/>
-      <c r="C190" s="12"/>
-      <c r="D190" s="12"/>
-      <c r="E190" s="12"/>
+      <c r="A190" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190" s="20">
+        <v>43838</v>
+      </c>
+      <c r="C190" s="12">
+        <v>0.85238850223430618</v>
+      </c>
+      <c r="D190" s="11"/>
+      <c r="E190" s="11"/>
       <c r="F190" s="2"/>
-      <c r="G190" s="13"/>
+      <c r="G190" s="12"/>
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
       <c r="J190" s="1"/>
@@ -7152,13 +7203,19 @@
       <c r="AA190" s="1"/>
     </row>
     <row r="191" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A191" s="5"/>
-      <c r="B191" s="10"/>
-      <c r="C191" s="12"/>
-      <c r="D191" s="12"/>
-      <c r="E191" s="12"/>
+      <c r="A191" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191" s="20">
+        <v>43839</v>
+      </c>
+      <c r="C191" s="12">
+        <v>0.96611090578671843</v>
+      </c>
+      <c r="D191" s="11"/>
+      <c r="E191" s="11"/>
       <c r="F191" s="2"/>
-      <c r="G191" s="13"/>
+      <c r="G191" s="12"/>
       <c r="H191" s="1"/>
       <c r="I191" s="1"/>
       <c r="J191" s="1"/>
@@ -7181,13 +7238,19 @@
       <c r="AA191" s="1"/>
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A192" s="5"/>
-      <c r="B192" s="10"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
-      <c r="E192" s="12"/>
+      <c r="A192" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B192" s="20">
+        <v>43840</v>
+      </c>
+      <c r="C192" s="12">
+        <v>0.98084890415942749</v>
+      </c>
+      <c r="D192" s="11"/>
+      <c r="E192" s="11"/>
       <c r="F192" s="2"/>
-      <c r="G192" s="13"/>
+      <c r="G192" s="12"/>
       <c r="H192" s="1"/>
       <c r="I192" s="1"/>
       <c r="J192" s="1"/>
@@ -7210,13 +7273,19 @@
       <c r="AA192" s="1"/>
     </row>
     <row r="193" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A193" s="5"/>
-      <c r="B193" s="10"/>
-      <c r="C193" s="12"/>
-      <c r="D193" s="12"/>
-      <c r="E193" s="12"/>
+      <c r="A193" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B193" s="20">
+        <v>43841</v>
+      </c>
+      <c r="C193" s="12">
+        <v>0.93404368956023198</v>
+      </c>
+      <c r="D193" s="11"/>
+      <c r="E193" s="11"/>
       <c r="F193" s="2"/>
-      <c r="G193" s="13"/>
+      <c r="G193" s="12"/>
       <c r="H193" s="1"/>
       <c r="I193" s="8"/>
       <c r="J193" s="1"/>
@@ -7239,13 +7308,19 @@
       <c r="AA193" s="1"/>
     </row>
     <row r="194" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A194" s="5"/>
-      <c r="B194" s="10"/>
-      <c r="C194" s="12"/>
-      <c r="D194" s="12"/>
-      <c r="E194" s="12"/>
+      <c r="A194" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B194" s="20">
+        <v>43842</v>
+      </c>
+      <c r="C194" s="12">
+        <v>0.42425815923245208</v>
+      </c>
+      <c r="D194" s="11"/>
+      <c r="E194" s="11"/>
       <c r="F194" s="2"/>
-      <c r="G194" s="13"/>
+      <c r="G194" s="12"/>
       <c r="H194" s="1"/>
       <c r="I194" s="1"/>
       <c r="J194" s="1"/>
@@ -7268,13 +7343,19 @@
       <c r="AA194" s="1"/>
     </row>
     <row r="195" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A195" s="5"/>
-      <c r="B195" s="10"/>
-      <c r="C195" s="12"/>
-      <c r="D195" s="12"/>
-      <c r="E195" s="12"/>
+      <c r="A195" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B195" s="20">
+        <v>43843</v>
+      </c>
+      <c r="C195" s="12">
+        <v>0.48139081874563455</v>
+      </c>
+      <c r="D195" s="11"/>
+      <c r="E195" s="11"/>
       <c r="F195" s="2"/>
-      <c r="G195" s="13"/>
+      <c r="G195" s="12"/>
       <c r="H195" s="1"/>
       <c r="I195" s="1"/>
       <c r="J195" s="1"/>
@@ -7297,13 +7378,19 @@
       <c r="AA195" s="1"/>
     </row>
     <row r="196" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A196" s="5"/>
-      <c r="B196" s="10"/>
-      <c r="C196" s="12"/>
-      <c r="D196" s="12"/>
-      <c r="E196" s="12"/>
+      <c r="A196" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B196" s="20">
+        <v>43844</v>
+      </c>
+      <c r="C196" s="12">
+        <v>0.45623720813878577</v>
+      </c>
+      <c r="D196" s="11"/>
+      <c r="E196" s="11"/>
       <c r="F196" s="2"/>
-      <c r="G196" s="13"/>
+      <c r="G196" s="12"/>
       <c r="H196" s="1"/>
       <c r="I196" s="1"/>
       <c r="J196" s="1"/>
@@ -7326,13 +7413,19 @@
       <c r="AA196" s="1"/>
     </row>
     <row r="197" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A197" s="5"/>
-      <c r="B197" s="10"/>
-      <c r="C197" s="12"/>
+      <c r="A197" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B197" s="20">
+        <v>43845</v>
+      </c>
+      <c r="C197" s="12">
+        <v>0.2717235831766574</v>
+      </c>
       <c r="D197" s="6"/>
-      <c r="E197" s="12"/>
+      <c r="E197" s="11"/>
       <c r="F197" s="2"/>
-      <c r="G197" s="13"/>
+      <c r="G197" s="12"/>
       <c r="H197" s="1"/>
       <c r="I197" s="1"/>
       <c r="J197" s="1"/>
@@ -7355,13 +7448,19 @@
       <c r="AA197" s="1"/>
     </row>
     <row r="198" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A198" s="5"/>
-      <c r="B198" s="10"/>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
+      <c r="A198" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B198" s="20">
+        <v>43846</v>
+      </c>
+      <c r="C198" s="12">
+        <v>0.28441329947158173</v>
+      </c>
+      <c r="D198" s="11"/>
+      <c r="E198" s="11"/>
       <c r="F198" s="2"/>
-      <c r="G198" s="13"/>
+      <c r="G198" s="12"/>
       <c r="H198" s="1"/>
       <c r="I198" s="1"/>
       <c r="J198" s="1"/>
@@ -7384,13 +7483,19 @@
       <c r="AA198" s="1"/>
     </row>
     <row r="199" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A199" s="5"/>
-      <c r="B199" s="10"/>
-      <c r="C199" s="12"/>
-      <c r="D199" s="12"/>
-      <c r="E199" s="12"/>
+      <c r="A199" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B199" s="20">
+        <v>43847</v>
+      </c>
+      <c r="C199" s="12">
+        <v>0.90300146455030594</v>
+      </c>
+      <c r="D199" s="11"/>
+      <c r="E199" s="11"/>
       <c r="F199" s="2"/>
-      <c r="G199" s="13"/>
+      <c r="G199" s="12"/>
       <c r="H199" s="1"/>
       <c r="I199" s="1"/>
       <c r="J199" s="1"/>
@@ -7413,13 +7518,19 @@
       <c r="AA199" s="1"/>
     </row>
     <row r="200" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A200" s="5"/>
-      <c r="B200" s="10"/>
-      <c r="C200" s="12"/>
-      <c r="D200" s="12"/>
-      <c r="E200" s="12"/>
+      <c r="A200" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B200" s="20">
+        <v>43848</v>
+      </c>
+      <c r="C200" s="12">
+        <v>0.27761389529552494</v>
+      </c>
+      <c r="D200" s="11"/>
+      <c r="E200" s="11"/>
       <c r="F200" s="2"/>
-      <c r="G200" s="13"/>
+      <c r="G200" s="12"/>
       <c r="H200" s="1"/>
       <c r="I200" s="8"/>
       <c r="J200" s="1"/>
@@ -7442,13 +7553,19 @@
       <c r="AA200" s="1"/>
     </row>
     <row r="201" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A201" s="5"/>
-      <c r="B201" s="10"/>
-      <c r="C201" s="12"/>
-      <c r="D201" s="12"/>
-      <c r="E201" s="12"/>
+      <c r="A201" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B201" s="20">
+        <v>43849</v>
+      </c>
+      <c r="C201" s="12">
+        <v>0.77246067387864881</v>
+      </c>
+      <c r="D201" s="11"/>
+      <c r="E201" s="11"/>
       <c r="F201" s="2"/>
-      <c r="G201" s="13"/>
+      <c r="G201" s="12"/>
       <c r="H201" s="1"/>
       <c r="I201" s="1"/>
       <c r="J201" s="1"/>
@@ -7471,13 +7588,19 @@
       <c r="AA201" s="1"/>
     </row>
     <row r="202" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A202" s="5"/>
-      <c r="B202" s="10"/>
-      <c r="C202" s="12"/>
-      <c r="D202" s="12"/>
-      <c r="E202" s="12"/>
+      <c r="A202" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B202" s="20">
+        <v>43850</v>
+      </c>
+      <c r="C202" s="12">
+        <v>0.93964874274740251</v>
+      </c>
+      <c r="D202" s="11"/>
+      <c r="E202" s="11"/>
       <c r="F202" s="2"/>
-      <c r="G202" s="13"/>
+      <c r="G202" s="12"/>
       <c r="H202" s="1"/>
       <c r="I202" s="1"/>
       <c r="J202" s="1"/>
@@ -7500,13 +7623,19 @@
       <c r="AA202" s="1"/>
     </row>
     <row r="203" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A203" s="5"/>
-      <c r="B203" s="10"/>
-      <c r="C203" s="12"/>
-      <c r="D203" s="12"/>
-      <c r="E203" s="12"/>
+      <c r="A203" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B203" s="20">
+        <v>43851</v>
+      </c>
+      <c r="C203" s="12">
+        <v>0.86392864326041663</v>
+      </c>
+      <c r="D203" s="11"/>
+      <c r="E203" s="11"/>
       <c r="F203" s="2"/>
-      <c r="G203" s="13"/>
+      <c r="G203" s="12"/>
       <c r="H203" s="1"/>
       <c r="I203" s="1"/>
       <c r="J203" s="1"/>
@@ -7529,13 +7658,19 @@
       <c r="AA203" s="1"/>
     </row>
     <row r="204" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A204" s="5"/>
-      <c r="B204" s="10"/>
-      <c r="C204" s="12"/>
-      <c r="D204" s="12"/>
-      <c r="E204" s="12"/>
+      <c r="A204" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B204" s="20">
+        <v>43852</v>
+      </c>
+      <c r="C204" s="12">
+        <v>0.98437012572970517</v>
+      </c>
+      <c r="D204" s="11"/>
+      <c r="E204" s="11"/>
       <c r="F204" s="2"/>
-      <c r="G204" s="13"/>
+      <c r="G204" s="12"/>
       <c r="H204" s="1"/>
       <c r="I204" s="1"/>
       <c r="J204" s="1"/>
@@ -7558,13 +7693,19 @@
       <c r="AA204" s="1"/>
     </row>
     <row r="205" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A205" s="5"/>
-      <c r="B205" s="10"/>
-      <c r="C205" s="12"/>
+      <c r="A205" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B205" s="20">
+        <v>43853</v>
+      </c>
+      <c r="C205" s="12">
+        <v>0.60605221946456156</v>
+      </c>
       <c r="D205" s="6"/>
-      <c r="E205" s="12"/>
+      <c r="E205" s="11"/>
       <c r="F205" s="2"/>
-      <c r="G205" s="13"/>
+      <c r="G205" s="12"/>
       <c r="H205" s="1"/>
       <c r="I205" s="1"/>
       <c r="J205" s="1"/>
@@ -7587,13 +7728,19 @@
       <c r="AA205" s="1"/>
     </row>
     <row r="206" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A206" s="5"/>
-      <c r="B206" s="10"/>
-      <c r="C206" s="12"/>
-      <c r="D206" s="12"/>
-      <c r="E206" s="12"/>
+      <c r="A206" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B206" s="20">
+        <v>43854</v>
+      </c>
+      <c r="C206" s="12">
+        <v>0.57221320279356391</v>
+      </c>
+      <c r="D206" s="11"/>
+      <c r="E206" s="11"/>
       <c r="F206" s="2"/>
-      <c r="G206" s="13"/>
+      <c r="G206" s="12"/>
       <c r="H206" s="1"/>
       <c r="I206" s="1"/>
       <c r="J206" s="1"/>
@@ -7616,13 +7763,19 @@
       <c r="AA206" s="1"/>
     </row>
     <row r="207" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A207" s="5"/>
-      <c r="B207" s="10"/>
-      <c r="C207" s="12"/>
-      <c r="D207" s="12"/>
-      <c r="E207" s="12"/>
+      <c r="A207" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B207" s="20">
+        <v>43855</v>
+      </c>
+      <c r="C207" s="12">
+        <v>0.5275164743382087</v>
+      </c>
+      <c r="D207" s="11"/>
+      <c r="E207" s="11"/>
       <c r="F207" s="2"/>
-      <c r="G207" s="13"/>
+      <c r="G207" s="12"/>
       <c r="H207" s="1"/>
       <c r="I207" s="8"/>
       <c r="J207" s="1"/>
@@ -7645,13 +7798,19 @@
       <c r="AA207" s="1"/>
     </row>
     <row r="208" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A208" s="5"/>
-      <c r="B208" s="10"/>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
+      <c r="A208" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B208" s="20">
+        <v>43856</v>
+      </c>
+      <c r="C208" s="12">
+        <v>0.22115980327512164</v>
+      </c>
+      <c r="D208" s="11"/>
+      <c r="E208" s="11"/>
       <c r="F208" s="2"/>
-      <c r="G208" s="13"/>
+      <c r="G208" s="12"/>
       <c r="H208" s="1"/>
       <c r="I208" s="1"/>
       <c r="J208" s="1"/>
@@ -7674,13 +7833,19 @@
       <c r="AA208" s="1"/>
     </row>
     <row r="209" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A209" s="5"/>
-      <c r="B209" s="10"/>
-      <c r="C209" s="12"/>
-      <c r="D209" s="12"/>
-      <c r="E209" s="12"/>
+      <c r="A209" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B209" s="20">
+        <v>43857</v>
+      </c>
+      <c r="C209" s="12">
+        <v>0.42316690286047715</v>
+      </c>
+      <c r="D209" s="11"/>
+      <c r="E209" s="11"/>
       <c r="F209" s="2"/>
-      <c r="G209" s="13"/>
+      <c r="G209" s="12"/>
       <c r="H209" s="1"/>
       <c r="I209" s="1"/>
       <c r="J209" s="1"/>
@@ -7703,13 +7868,19 @@
       <c r="AA209" s="1"/>
     </row>
     <row r="210" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A210" s="5"/>
-      <c r="B210" s="10"/>
-      <c r="C210" s="12"/>
-      <c r="D210" s="12"/>
-      <c r="E210" s="12"/>
+      <c r="A210" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B210" s="20">
+        <v>43858</v>
+      </c>
+      <c r="C210" s="12">
+        <v>0.45025320279278008</v>
+      </c>
+      <c r="D210" s="11"/>
+      <c r="E210" s="11"/>
       <c r="F210" s="2"/>
-      <c r="G210" s="13"/>
+      <c r="G210" s="12"/>
       <c r="H210" s="1"/>
       <c r="I210" s="1"/>
       <c r="J210" s="1"/>
@@ -7732,13 +7903,19 @@
       <c r="AA210" s="1"/>
     </row>
     <row r="211" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A211" s="5"/>
-      <c r="B211" s="10"/>
-      <c r="C211" s="12"/>
-      <c r="D211" s="12"/>
-      <c r="E211" s="12"/>
+      <c r="A211" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B211" s="20">
+        <v>43859</v>
+      </c>
+      <c r="C211" s="12">
+        <v>0.66695528574938912</v>
+      </c>
+      <c r="D211" s="11"/>
+      <c r="E211" s="11"/>
       <c r="F211" s="2"/>
-      <c r="G211" s="13"/>
+      <c r="G211" s="12"/>
       <c r="H211" s="1"/>
       <c r="I211" s="1"/>
       <c r="J211" s="1"/>
@@ -7761,13 +7938,19 @@
       <c r="AA211" s="1"/>
     </row>
     <row r="212" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A212" s="5"/>
-      <c r="B212" s="10"/>
-      <c r="C212" s="12"/>
-      <c r="D212" s="12"/>
-      <c r="E212" s="12"/>
+      <c r="A212" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B212" s="20">
+        <v>43860</v>
+      </c>
+      <c r="C212" s="12">
+        <v>0.44038197246677513</v>
+      </c>
+      <c r="D212" s="11"/>
+      <c r="E212" s="11"/>
       <c r="F212" s="2"/>
-      <c r="G212" s="13"/>
+      <c r="G212" s="12"/>
       <c r="H212" s="1"/>
       <c r="I212" s="1"/>
       <c r="J212" s="1"/>
@@ -7790,13 +7973,19 @@
       <c r="AA212" s="1"/>
     </row>
     <row r="213" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A213" s="5"/>
-      <c r="B213" s="10"/>
-      <c r="C213" s="12"/>
+      <c r="A213" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B213" s="20">
+        <v>43861</v>
+      </c>
+      <c r="C213" s="12">
+        <v>0.23573874470319889</v>
+      </c>
       <c r="D213" s="6"/>
-      <c r="E213" s="12"/>
+      <c r="E213" s="11"/>
       <c r="F213" s="2"/>
-      <c r="G213" s="13"/>
+      <c r="G213" s="12"/>
       <c r="H213" s="1"/>
       <c r="I213" s="1"/>
       <c r="J213" s="1"/>
@@ -7819,13 +8008,19 @@
       <c r="AA213" s="1"/>
     </row>
     <row r="214" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A214" s="5"/>
-      <c r="B214" s="10"/>
-      <c r="C214" s="12"/>
-      <c r="D214" s="12"/>
-      <c r="E214" s="12"/>
+      <c r="A214" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B214" s="20">
+        <v>43862</v>
+      </c>
+      <c r="C214" s="12">
+        <v>0.44878046896181428</v>
+      </c>
+      <c r="D214" s="11"/>
+      <c r="E214" s="11"/>
       <c r="F214" s="2"/>
-      <c r="G214" s="13"/>
+      <c r="G214" s="12"/>
       <c r="H214" s="1"/>
       <c r="I214" s="8"/>
       <c r="J214" s="1"/>
@@ -7848,13 +8043,19 @@
       <c r="AA214" s="1"/>
     </row>
     <row r="215" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A215" s="5"/>
-      <c r="B215" s="10"/>
-      <c r="C215" s="12"/>
-      <c r="D215" s="12"/>
-      <c r="E215" s="12"/>
+      <c r="A215" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B215" s="20">
+        <v>43863</v>
+      </c>
+      <c r="C215" s="12">
+        <v>0.5164434397051384</v>
+      </c>
+      <c r="D215" s="11"/>
+      <c r="E215" s="11"/>
       <c r="F215" s="2"/>
-      <c r="G215" s="13"/>
+      <c r="G215" s="12"/>
       <c r="H215" s="1"/>
       <c r="I215" s="1"/>
       <c r="J215" s="1"/>
@@ -7877,13 +8078,19 @@
       <c r="AA215" s="1"/>
     </row>
     <row r="216" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A216" s="5"/>
-      <c r="B216" s="10"/>
-      <c r="C216" s="12"/>
-      <c r="D216" s="12"/>
-      <c r="E216" s="12"/>
+      <c r="A216" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B216" s="20">
+        <v>43864</v>
+      </c>
+      <c r="C216" s="12">
+        <v>0.77105482533125547</v>
+      </c>
+      <c r="D216" s="11"/>
+      <c r="E216" s="11"/>
       <c r="F216" s="2"/>
-      <c r="G216" s="13"/>
+      <c r="G216" s="12"/>
       <c r="H216" s="1"/>
       <c r="I216" s="1"/>
       <c r="J216" s="1"/>
@@ -7906,13 +8113,19 @@
       <c r="AA216" s="1"/>
     </row>
     <row r="217" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A217" s="5"/>
-      <c r="B217" s="10"/>
-      <c r="C217" s="12"/>
-      <c r="D217" s="12"/>
-      <c r="E217" s="12"/>
+      <c r="A217" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B217" s="20">
+        <v>43865</v>
+      </c>
+      <c r="C217" s="12">
+        <v>0.69817928637888649</v>
+      </c>
+      <c r="D217" s="11"/>
+      <c r="E217" s="11"/>
       <c r="F217" s="2"/>
-      <c r="G217" s="13"/>
+      <c r="G217" s="12"/>
       <c r="H217" s="1"/>
       <c r="I217" s="1"/>
       <c r="J217" s="1"/>
@@ -7935,13 +8148,19 @@
       <c r="AA217" s="1"/>
     </row>
     <row r="218" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A218" s="5"/>
-      <c r="B218" s="10"/>
-      <c r="C218" s="12"/>
-      <c r="D218" s="12"/>
-      <c r="E218" s="12"/>
+      <c r="A218" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B218" s="20">
+        <v>43866</v>
+      </c>
+      <c r="C218" s="12">
+        <v>0.44218596499206991</v>
+      </c>
+      <c r="D218" s="11"/>
+      <c r="E218" s="11"/>
       <c r="F218" s="2"/>
-      <c r="G218" s="13"/>
+      <c r="G218" s="12"/>
       <c r="H218" s="1"/>
       <c r="I218" s="1"/>
       <c r="J218" s="1"/>
@@ -7964,13 +8183,19 @@
       <c r="AA218" s="1"/>
     </row>
     <row r="219" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A219" s="5"/>
-      <c r="B219" s="10"/>
-      <c r="C219" s="12"/>
-      <c r="D219" s="12"/>
-      <c r="E219" s="12"/>
+      <c r="A219" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B219" s="20">
+        <v>43867</v>
+      </c>
+      <c r="C219" s="12">
+        <v>0.31778622674291679</v>
+      </c>
+      <c r="D219" s="11"/>
+      <c r="E219" s="11"/>
       <c r="F219" s="2"/>
-      <c r="G219" s="13"/>
+      <c r="G219" s="12"/>
       <c r="H219" s="1"/>
       <c r="I219" s="1"/>
       <c r="J219" s="1"/>
@@ -7993,13 +8218,19 @@
       <c r="AA219" s="1"/>
     </row>
     <row r="220" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A220" s="5"/>
-      <c r="B220" s="10"/>
-      <c r="C220" s="12"/>
-      <c r="D220" s="12"/>
-      <c r="E220" s="12"/>
+      <c r="A220" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B220" s="20">
+        <v>43868</v>
+      </c>
+      <c r="C220" s="12">
+        <v>0.31203072720546976</v>
+      </c>
+      <c r="D220" s="11"/>
+      <c r="E220" s="11"/>
       <c r="F220" s="2"/>
-      <c r="G220" s="13"/>
+      <c r="G220" s="12"/>
       <c r="H220" s="1"/>
       <c r="I220" s="1"/>
       <c r="J220" s="1"/>
@@ -8022,13 +8253,19 @@
       <c r="AA220" s="1"/>
     </row>
     <row r="221" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A221" s="5"/>
-      <c r="B221" s="10"/>
-      <c r="C221" s="12"/>
+      <c r="A221" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B221" s="20">
+        <v>43869</v>
+      </c>
+      <c r="C221" s="12">
+        <v>0.44336176727595827</v>
+      </c>
       <c r="D221" s="6"/>
-      <c r="E221" s="12"/>
+      <c r="E221" s="11"/>
       <c r="F221" s="2"/>
-      <c r="G221" s="13"/>
+      <c r="G221" s="12"/>
       <c r="H221" s="1"/>
       <c r="I221" s="8"/>
       <c r="J221" s="1"/>
@@ -8051,9 +8288,15 @@
       <c r="AA221" s="1"/>
     </row>
     <row r="222" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A222" s="17"/>
-      <c r="B222" s="1"/>
-      <c r="C222" s="8"/>
+      <c r="A222" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B222" s="8">
+        <v>43870</v>
+      </c>
+      <c r="C222" s="2">
+        <v>0.71734970443890256</v>
+      </c>
       <c r="D222" s="6"/>
       <c r="E222" s="8"/>
       <c r="F222" s="2"/>
@@ -8080,9 +8323,15 @@
       <c r="AA222" s="1"/>
     </row>
     <row r="223" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A223" s="17"/>
-      <c r="B223" s="1"/>
-      <c r="C223" s="8"/>
+      <c r="A223" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B223" s="8">
+        <v>43871</v>
+      </c>
+      <c r="C223" s="2">
+        <v>0.33626786819827198</v>
+      </c>
       <c r="D223" s="6"/>
       <c r="E223" s="8"/>
       <c r="F223" s="2"/>
@@ -8109,9 +8358,15 @@
       <c r="AA223" s="1"/>
     </row>
     <row r="224" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A224" s="17"/>
-      <c r="B224" s="1"/>
-      <c r="C224" s="8"/>
+      <c r="A224" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B224" s="8">
+        <v>43872</v>
+      </c>
+      <c r="C224" s="2">
+        <v>0.88070777457483407</v>
+      </c>
       <c r="D224" s="6"/>
       <c r="E224" s="8"/>
       <c r="F224" s="2"/>
@@ -8138,15 +8393,21 @@
       <c r="AA224" s="1"/>
     </row>
     <row r="225" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A225" s="17"/>
-      <c r="B225" s="1"/>
-      <c r="C225" s="8"/>
+      <c r="A225" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B225" s="8">
+        <v>43873</v>
+      </c>
+      <c r="C225" s="2">
+        <v>0.60249535453517367</v>
+      </c>
       <c r="D225" s="6"/>
       <c r="E225" s="8"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
       <c r="H225" s="1"/>
-      <c r="I225" s="18"/>
+      <c r="I225" s="17"/>
       <c r="J225" s="1"/>
       <c r="K225" s="1"/>
       <c r="L225" s="1"/>
@@ -8167,15 +8428,21 @@
       <c r="AA225" s="1"/>
     </row>
     <row r="226" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A226" s="17"/>
-      <c r="B226" s="1"/>
-      <c r="C226" s="8"/>
+      <c r="A226" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B226" s="8">
+        <v>43874</v>
+      </c>
+      <c r="C226" s="2">
+        <v>0.51325173436108629</v>
+      </c>
       <c r="D226" s="6"/>
       <c r="E226" s="8"/>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
       <c r="H226" s="1"/>
-      <c r="I226" s="18"/>
+      <c r="I226" s="17"/>
       <c r="J226" s="1"/>
       <c r="K226" s="1"/>
       <c r="L226" s="1"/>
@@ -8196,15 +8463,21 @@
       <c r="AA226" s="1"/>
     </row>
     <row r="227" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A227" s="17"/>
-      <c r="B227" s="1"/>
-      <c r="C227" s="8"/>
+      <c r="A227" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B227" s="8">
+        <v>43875</v>
+      </c>
+      <c r="C227" s="2">
+        <v>0.33143658889543115</v>
+      </c>
       <c r="D227" s="6"/>
       <c r="E227" s="8"/>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
       <c r="H227" s="1"/>
-      <c r="I227" s="18"/>
+      <c r="I227" s="17"/>
       <c r="J227" s="1"/>
       <c r="K227" s="1"/>
       <c r="L227" s="1"/>
@@ -8225,15 +8498,21 @@
       <c r="AA227" s="1"/>
     </row>
     <row r="228" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A228" s="17"/>
-      <c r="B228" s="1"/>
-      <c r="C228" s="8"/>
+      <c r="A228" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B228" s="8">
+        <v>43876</v>
+      </c>
+      <c r="C228" s="2">
+        <v>0.31736631917186747</v>
+      </c>
       <c r="D228" s="6"/>
       <c r="E228" s="8"/>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
       <c r="H228" s="1"/>
-      <c r="I228" s="18"/>
+      <c r="I228" s="17"/>
       <c r="J228" s="1"/>
       <c r="K228" s="1"/>
       <c r="L228" s="1"/>
@@ -8254,15 +8533,21 @@
       <c r="AA228" s="1"/>
     </row>
     <row r="229" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A229" s="17"/>
-      <c r="B229" s="1"/>
-      <c r="C229" s="8"/>
+      <c r="A229" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B229" s="8">
+        <v>43877</v>
+      </c>
+      <c r="C229" s="2">
+        <v>0.82818568806079929</v>
+      </c>
       <c r="D229" s="6"/>
       <c r="E229" s="8"/>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
       <c r="H229" s="1"/>
-      <c r="I229" s="18"/>
+      <c r="I229" s="17"/>
       <c r="J229" s="1"/>
       <c r="K229" s="1"/>
       <c r="L229" s="1"/>
@@ -8283,15 +8568,21 @@
       <c r="AA229" s="1"/>
     </row>
     <row r="230" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A230" s="17"/>
-      <c r="B230" s="1"/>
-      <c r="C230" s="8"/>
+      <c r="A230" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B230" s="8">
+        <v>43878</v>
+      </c>
+      <c r="C230" s="2">
+        <v>0.34486345185834222</v>
+      </c>
       <c r="D230" s="6"/>
       <c r="E230" s="8"/>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
       <c r="H230" s="1"/>
-      <c r="I230" s="18"/>
+      <c r="I230" s="17"/>
       <c r="J230" s="1"/>
       <c r="K230" s="1"/>
       <c r="L230" s="1"/>
@@ -8312,15 +8603,21 @@
       <c r="AA230" s="1"/>
     </row>
     <row r="231" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A231" s="17"/>
-      <c r="B231" s="1"/>
-      <c r="C231" s="8"/>
+      <c r="A231" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B231" s="8">
+        <v>43879</v>
+      </c>
+      <c r="C231" s="2">
+        <v>0.38532428984939199</v>
+      </c>
       <c r="D231" s="6"/>
       <c r="E231" s="8"/>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
       <c r="H231" s="1"/>
-      <c r="I231" s="18"/>
+      <c r="I231" s="17"/>
       <c r="J231" s="1"/>
       <c r="K231" s="1"/>
       <c r="L231" s="1"/>
@@ -8341,15 +8638,21 @@
       <c r="AA231" s="1"/>
     </row>
     <row r="232" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A232" s="17"/>
-      <c r="B232" s="1"/>
-      <c r="C232" s="8"/>
+      <c r="A232" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B232" s="8">
+        <v>43880</v>
+      </c>
+      <c r="C232" s="2">
+        <v>0.50367650967035738</v>
+      </c>
       <c r="D232" s="6"/>
       <c r="E232" s="8"/>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
       <c r="H232" s="1"/>
-      <c r="I232" s="18"/>
+      <c r="I232" s="17"/>
       <c r="J232" s="1"/>
       <c r="K232" s="1"/>
       <c r="L232" s="1"/>
@@ -8370,15 +8673,21 @@
       <c r="AA232" s="1"/>
     </row>
     <row r="233" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A233" s="17"/>
-      <c r="B233" s="1"/>
-      <c r="C233" s="8"/>
+      <c r="A233" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B233" s="8">
+        <v>43881</v>
+      </c>
+      <c r="C233" s="2">
+        <v>0.66933587790918525</v>
+      </c>
       <c r="D233" s="6"/>
       <c r="E233" s="8"/>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
       <c r="H233" s="1"/>
-      <c r="I233" s="18"/>
+      <c r="I233" s="17"/>
       <c r="J233" s="1"/>
       <c r="K233" s="1"/>
       <c r="L233" s="1"/>
@@ -8399,15 +8708,21 @@
       <c r="AA233" s="1"/>
     </row>
     <row r="234" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A234" s="17"/>
-      <c r="B234" s="1"/>
-      <c r="C234" s="8"/>
+      <c r="A234" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B234" s="8">
+        <v>43882</v>
+      </c>
+      <c r="C234" s="2">
+        <v>0.54505615121065176</v>
+      </c>
       <c r="D234" s="6"/>
       <c r="E234" s="8"/>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
       <c r="H234" s="1"/>
-      <c r="I234" s="18"/>
+      <c r="I234" s="17"/>
       <c r="J234" s="1"/>
       <c r="K234" s="1"/>
       <c r="L234" s="1"/>
@@ -8428,15 +8743,21 @@
       <c r="AA234" s="1"/>
     </row>
     <row r="235" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A235" s="17"/>
-      <c r="B235" s="1"/>
-      <c r="C235" s="8"/>
+      <c r="A235" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B235" s="8">
+        <v>43883</v>
+      </c>
+      <c r="C235" s="2">
+        <v>0.45640725992211845</v>
+      </c>
       <c r="D235" s="6"/>
       <c r="E235" s="8"/>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
       <c r="H235" s="1"/>
-      <c r="I235" s="18"/>
+      <c r="I235" s="17"/>
       <c r="J235" s="1"/>
       <c r="K235" s="1"/>
       <c r="L235" s="1"/>
@@ -8457,15 +8778,21 @@
       <c r="AA235" s="1"/>
     </row>
     <row r="236" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A236" s="17"/>
-      <c r="B236" s="1"/>
-      <c r="C236" s="8"/>
+      <c r="A236" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B236" s="8">
+        <v>43884</v>
+      </c>
+      <c r="C236" s="2">
+        <v>0.49802096950743457</v>
+      </c>
       <c r="D236" s="6"/>
       <c r="E236" s="8"/>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
       <c r="H236" s="1"/>
-      <c r="I236" s="18"/>
+      <c r="I236" s="17"/>
       <c r="J236" s="1"/>
       <c r="K236" s="1"/>
       <c r="L236" s="1"/>
@@ -8486,15 +8813,21 @@
       <c r="AA236" s="1"/>
     </row>
     <row r="237" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A237" s="17"/>
-      <c r="B237" s="1"/>
-      <c r="C237" s="8"/>
+      <c r="A237" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237" s="8">
+        <v>43885</v>
+      </c>
+      <c r="C237" s="2">
+        <v>0.33544723889545763</v>
+      </c>
       <c r="D237" s="6"/>
       <c r="E237" s="8"/>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
       <c r="H237" s="1"/>
-      <c r="I237" s="18"/>
+      <c r="I237" s="17"/>
       <c r="J237" s="1"/>
       <c r="K237" s="1"/>
       <c r="L237" s="1"/>
@@ -8515,15 +8848,21 @@
       <c r="AA237" s="1"/>
     </row>
     <row r="238" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A238" s="17"/>
-      <c r="B238" s="1"/>
-      <c r="C238" s="8"/>
+      <c r="A238" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B238" s="8">
+        <v>43886</v>
+      </c>
+      <c r="C238" s="2">
+        <v>0.40252980064594229</v>
+      </c>
       <c r="D238" s="6"/>
       <c r="E238" s="8"/>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
       <c r="H238" s="1"/>
-      <c r="I238" s="18"/>
+      <c r="I238" s="17"/>
       <c r="J238" s="1"/>
       <c r="K238" s="1"/>
       <c r="L238" s="1"/>
@@ -8544,15 +8883,21 @@
       <c r="AA238" s="1"/>
     </row>
     <row r="239" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A239" s="17"/>
-      <c r="B239" s="1"/>
-      <c r="C239" s="8"/>
+      <c r="A239" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B239" s="8">
+        <v>43887</v>
+      </c>
+      <c r="C239" s="2">
+        <v>0.73340102318558098</v>
+      </c>
       <c r="D239" s="6"/>
       <c r="E239" s="8"/>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
       <c r="H239" s="1"/>
-      <c r="I239" s="18"/>
+      <c r="I239" s="17"/>
       <c r="J239" s="1"/>
       <c r="K239" s="1"/>
       <c r="L239" s="1"/>
@@ -8573,15 +8918,21 @@
       <c r="AA239" s="1"/>
     </row>
     <row r="240" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A240" s="17"/>
-      <c r="B240" s="1"/>
-      <c r="C240" s="8"/>
+      <c r="A240" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B240" s="8">
+        <v>43888</v>
+      </c>
+      <c r="C240" s="2">
+        <v>0.9595337826708995</v>
+      </c>
       <c r="D240" s="6"/>
       <c r="E240" s="8"/>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
       <c r="H240" s="1"/>
-      <c r="I240" s="18"/>
+      <c r="I240" s="17"/>
       <c r="J240" s="1"/>
       <c r="K240" s="1"/>
       <c r="L240" s="1"/>
@@ -8602,15 +8953,21 @@
       <c r="AA240" s="1"/>
     </row>
     <row r="241" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A241" s="17"/>
-      <c r="B241" s="1"/>
-      <c r="C241" s="8"/>
+      <c r="A241" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B241" s="8">
+        <v>43889</v>
+      </c>
+      <c r="C241" s="2">
+        <v>0.8630839017612868</v>
+      </c>
       <c r="D241" s="6"/>
       <c r="E241" s="8"/>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
       <c r="H241" s="1"/>
-      <c r="I241" s="18"/>
+      <c r="I241" s="17"/>
       <c r="J241" s="1"/>
       <c r="K241" s="1"/>
       <c r="L241" s="1"/>
@@ -8631,15 +8988,21 @@
       <c r="AA241" s="1"/>
     </row>
     <row r="242" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A242" s="17"/>
-      <c r="B242" s="1"/>
-      <c r="C242" s="8"/>
+      <c r="A242" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B242" s="8">
+        <v>43890</v>
+      </c>
+      <c r="C242" s="2">
+        <v>0.72541684438155285</v>
+      </c>
       <c r="D242" s="6"/>
       <c r="E242" s="8"/>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
       <c r="H242" s="1"/>
-      <c r="I242" s="18"/>
+      <c r="I242" s="17"/>
       <c r="J242" s="1"/>
       <c r="K242" s="1"/>
       <c r="L242" s="1"/>
@@ -8660,15 +9023,21 @@
       <c r="AA242" s="1"/>
     </row>
     <row r="243" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A243" s="17"/>
-      <c r="B243" s="1"/>
-      <c r="C243" s="8"/>
+      <c r="A243" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B243" s="8">
+        <v>43891</v>
+      </c>
+      <c r="C243" s="2">
+        <v>0.40735996971992133</v>
+      </c>
       <c r="D243" s="6"/>
       <c r="E243" s="8"/>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
       <c r="H243" s="1"/>
-      <c r="I243" s="18"/>
+      <c r="I243" s="17"/>
       <c r="J243" s="1"/>
       <c r="K243" s="1"/>
       <c r="L243" s="1"/>
@@ -8689,9 +9058,15 @@
       <c r="AA243" s="1"/>
     </row>
     <row r="244" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A244" s="17"/>
-      <c r="B244" s="1"/>
-      <c r="C244" s="8"/>
+      <c r="A244" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B244" s="8">
+        <v>43892</v>
+      </c>
+      <c r="C244" s="2">
+        <v>0.48057424119452102</v>
+      </c>
       <c r="D244" s="6"/>
       <c r="E244" s="8"/>
       <c r="F244" s="2"/>
@@ -8718,9 +9093,15 @@
       <c r="AA244" s="1"/>
     </row>
     <row r="245" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A245" s="17"/>
-      <c r="B245" s="1"/>
-      <c r="C245" s="8"/>
+      <c r="A245" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B245" s="8">
+        <v>43893</v>
+      </c>
+      <c r="C245" s="2">
+        <v>0.89805957366983336</v>
+      </c>
       <c r="D245" s="6"/>
       <c r="E245" s="8"/>
       <c r="F245" s="2"/>
@@ -8747,9 +9128,15 @@
       <c r="AA245" s="1"/>
     </row>
     <row r="246" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A246" s="17"/>
-      <c r="B246" s="1"/>
-      <c r="C246" s="8"/>
+      <c r="A246" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B246" s="8">
+        <v>43894</v>
+      </c>
+      <c r="C246" s="2">
+        <v>0.41386708552459267</v>
+      </c>
       <c r="D246" s="6"/>
       <c r="E246" s="8"/>
       <c r="F246" s="2"/>
@@ -8776,15 +9163,21 @@
       <c r="AA246" s="1"/>
     </row>
     <row r="247" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A247" s="17"/>
-      <c r="B247" s="1"/>
-      <c r="C247" s="8"/>
+      <c r="A247" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B247" s="8">
+        <v>43895</v>
+      </c>
+      <c r="C247" s="2">
+        <v>0.44988657311214203</v>
+      </c>
       <c r="D247" s="6"/>
       <c r="E247" s="8"/>
       <c r="F247" s="2"/>
       <c r="G247" s="2"/>
       <c r="H247" s="1"/>
-      <c r="I247" s="18"/>
+      <c r="I247" s="17"/>
       <c r="J247" s="1"/>
       <c r="K247" s="1"/>
       <c r="L247" s="1"/>
@@ -8805,15 +9198,21 @@
       <c r="AA247" s="1"/>
     </row>
     <row r="248" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A248" s="17"/>
-      <c r="B248" s="1"/>
-      <c r="C248" s="8"/>
+      <c r="A248" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B248" s="8">
+        <v>43896</v>
+      </c>
+      <c r="C248" s="2">
+        <v>0.27348533107205925</v>
+      </c>
       <c r="D248" s="6"/>
       <c r="E248" s="8"/>
       <c r="F248" s="2"/>
       <c r="G248" s="2"/>
       <c r="H248" s="1"/>
-      <c r="I248" s="18"/>
+      <c r="I248" s="17"/>
       <c r="J248" s="1"/>
       <c r="K248" s="1"/>
       <c r="L248" s="1"/>
@@ -8834,15 +9233,21 @@
       <c r="AA248" s="1"/>
     </row>
     <row r="249" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A249" s="17"/>
-      <c r="B249" s="1"/>
-      <c r="C249" s="8"/>
+      <c r="A249" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B249" s="8">
+        <v>43897</v>
+      </c>
+      <c r="C249" s="2">
+        <v>0.86031879011421541</v>
+      </c>
       <c r="D249" s="6"/>
       <c r="E249" s="8"/>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
       <c r="H249" s="1"/>
-      <c r="I249" s="18"/>
+      <c r="I249" s="17"/>
       <c r="J249" s="1"/>
       <c r="K249" s="1"/>
       <c r="L249" s="1"/>
@@ -8863,15 +9268,21 @@
       <c r="AA249" s="1"/>
     </row>
     <row r="250" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A250" s="17"/>
-      <c r="B250" s="1"/>
-      <c r="C250" s="8"/>
+      <c r="A250" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B250" s="8">
+        <v>43898</v>
+      </c>
+      <c r="C250" s="2">
+        <v>0.78197659129852082</v>
+      </c>
       <c r="D250" s="6"/>
       <c r="E250" s="8"/>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
       <c r="H250" s="1"/>
-      <c r="I250" s="18"/>
+      <c r="I250" s="17"/>
       <c r="J250" s="1"/>
       <c r="K250" s="1"/>
       <c r="L250" s="1"/>
@@ -8892,15 +9303,21 @@
       <c r="AA250" s="1"/>
     </row>
     <row r="251" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A251" s="17"/>
-      <c r="B251" s="1"/>
-      <c r="C251" s="8"/>
+      <c r="A251" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B251" s="8">
+        <v>43899</v>
+      </c>
+      <c r="C251" s="2">
+        <v>0.98951256833494028</v>
+      </c>
       <c r="D251" s="6"/>
       <c r="E251" s="8"/>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
       <c r="H251" s="1"/>
-      <c r="I251" s="18"/>
+      <c r="I251" s="17"/>
       <c r="J251" s="1"/>
       <c r="K251" s="1"/>
       <c r="L251" s="1"/>
@@ -8921,15 +9338,21 @@
       <c r="AA251" s="1"/>
     </row>
     <row r="252" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A252" s="17"/>
-      <c r="B252" s="1"/>
-      <c r="C252" s="8"/>
+      <c r="A252" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B252" s="8">
+        <v>43900</v>
+      </c>
+      <c r="C252" s="2">
+        <v>0.21386138229334592</v>
+      </c>
       <c r="D252" s="6"/>
       <c r="E252" s="8"/>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
       <c r="H252" s="1"/>
-      <c r="I252" s="18"/>
+      <c r="I252" s="17"/>
       <c r="J252" s="1"/>
       <c r="K252" s="1"/>
       <c r="L252" s="1"/>
@@ -8950,15 +9373,21 @@
       <c r="AA252" s="1"/>
     </row>
     <row r="253" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A253" s="17"/>
-      <c r="B253" s="1"/>
-      <c r="C253" s="8"/>
+      <c r="A253" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B253" s="8">
+        <v>43901</v>
+      </c>
+      <c r="C253" s="2">
+        <v>0.29101769627677554</v>
+      </c>
       <c r="D253" s="6"/>
       <c r="E253" s="8"/>
       <c r="F253" s="2"/>
       <c r="G253" s="2"/>
       <c r="H253" s="1"/>
-      <c r="I253" s="18"/>
+      <c r="I253" s="17"/>
       <c r="J253" s="1"/>
       <c r="K253" s="1"/>
       <c r="L253" s="1"/>
@@ -8979,15 +9408,21 @@
       <c r="AA253" s="1"/>
     </row>
     <row r="254" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A254" s="17"/>
-      <c r="B254" s="1"/>
-      <c r="C254" s="8"/>
+      <c r="A254" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B254" s="8">
+        <v>43902</v>
+      </c>
+      <c r="C254" s="2">
+        <v>0.18583324702568899</v>
+      </c>
       <c r="D254" s="6"/>
       <c r="E254" s="8"/>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
       <c r="H254" s="1"/>
-      <c r="I254" s="18"/>
+      <c r="I254" s="17"/>
       <c r="J254" s="1"/>
       <c r="K254" s="1"/>
       <c r="L254" s="1"/>
@@ -9008,15 +9443,21 @@
       <c r="AA254" s="1"/>
     </row>
     <row r="255" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A255" s="17"/>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
+      <c r="A255" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B255" s="8">
+        <v>43903</v>
+      </c>
+      <c r="C255" s="2">
+        <v>0.1205451413653636</v>
+      </c>
       <c r="D255" s="6"/>
       <c r="E255" s="8"/>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
       <c r="H255" s="1"/>
-      <c r="I255" s="18"/>
+      <c r="I255" s="17"/>
       <c r="J255" s="1"/>
       <c r="K255" s="1"/>
       <c r="L255" s="1"/>
@@ -9037,15 +9478,21 @@
       <c r="AA255" s="1"/>
     </row>
     <row r="256" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A256" s="17"/>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
+      <c r="A256" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B256" s="8">
+        <v>43904</v>
+      </c>
+      <c r="C256" s="2">
+        <v>0.27522113396730774</v>
+      </c>
       <c r="D256" s="6"/>
       <c r="E256" s="8"/>
       <c r="F256" s="2"/>
       <c r="G256" s="2"/>
       <c r="H256" s="1"/>
-      <c r="I256" s="18"/>
+      <c r="I256" s="17"/>
       <c r="J256" s="1"/>
       <c r="K256" s="1"/>
       <c r="L256" s="1"/>
@@ -9066,15 +9513,21 @@
       <c r="AA256" s="1"/>
     </row>
     <row r="257" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A257" s="17"/>
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
+      <c r="A257" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B257" s="8">
+        <v>43905</v>
+      </c>
+      <c r="C257" s="2">
+        <v>0.3832110713152988</v>
+      </c>
       <c r="D257" s="6"/>
       <c r="E257" s="8"/>
       <c r="F257" s="2"/>
       <c r="G257" s="2"/>
       <c r="H257" s="1"/>
-      <c r="I257" s="18"/>
+      <c r="I257" s="17"/>
       <c r="J257" s="1"/>
       <c r="K257" s="1"/>
       <c r="L257" s="1"/>
@@ -9095,15 +9548,21 @@
       <c r="AA257" s="1"/>
     </row>
     <row r="258" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A258" s="17"/>
-      <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
+      <c r="A258" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B258" s="8">
+        <v>43906</v>
+      </c>
+      <c r="C258" s="2">
+        <v>0.14297268753756953</v>
+      </c>
       <c r="D258" s="6"/>
       <c r="E258" s="8"/>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
-      <c r="H258" s="18"/>
-      <c r="I258" s="18"/>
+      <c r="H258" s="17"/>
+      <c r="I258" s="17"/>
       <c r="J258" s="1"/>
       <c r="K258" s="1"/>
       <c r="L258" s="1"/>
@@ -9124,15 +9583,21 @@
       <c r="AA258" s="1"/>
     </row>
     <row r="259" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A259" s="17"/>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
+      <c r="A259" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B259" s="8">
+        <v>43907</v>
+      </c>
+      <c r="C259" s="2">
+        <v>0.42950476899311546</v>
+      </c>
       <c r="D259" s="6"/>
       <c r="E259" s="8"/>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
-      <c r="H259" s="18"/>
-      <c r="I259" s="18"/>
+      <c r="H259" s="17"/>
+      <c r="I259" s="17"/>
       <c r="J259" s="1"/>
       <c r="K259" s="1"/>
       <c r="L259" s="1"/>
@@ -9153,15 +9618,21 @@
       <c r="AA259" s="1"/>
     </row>
     <row r="260" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A260" s="17"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
+      <c r="A260" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B260" s="8">
+        <v>43908</v>
+      </c>
+      <c r="C260" s="2">
+        <v>0.30967370562673013</v>
+      </c>
       <c r="D260" s="6"/>
       <c r="E260" s="8"/>
       <c r="F260" s="2"/>
       <c r="G260" s="2"/>
-      <c r="H260" s="18"/>
-      <c r="I260" s="18"/>
+      <c r="H260" s="17"/>
+      <c r="I260" s="17"/>
       <c r="J260" s="1"/>
       <c r="K260" s="1"/>
       <c r="L260" s="1"/>
@@ -9182,15 +9653,21 @@
       <c r="AA260" s="1"/>
     </row>
     <row r="261" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A261" s="17"/>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="A261" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B261" s="8">
+        <v>43909</v>
+      </c>
+      <c r="C261" s="2">
+        <v>0.14125957734242853</v>
+      </c>
       <c r="D261" s="6"/>
       <c r="E261" s="8"/>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
-      <c r="H261" s="18"/>
-      <c r="I261" s="18"/>
+      <c r="H261" s="17"/>
+      <c r="I261" s="17"/>
       <c r="J261" s="1"/>
       <c r="K261" s="1"/>
       <c r="L261" s="1"/>
@@ -9211,15 +9688,21 @@
       <c r="AA261" s="1"/>
     </row>
     <row r="262" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A262" s="17"/>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
+      <c r="A262" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B262" s="8">
+        <v>43910</v>
+      </c>
+      <c r="C262" s="2">
+        <v>0.22668808410896563</v>
+      </c>
       <c r="D262" s="6"/>
       <c r="E262" s="8"/>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
-      <c r="H262" s="18"/>
-      <c r="I262" s="18"/>
+      <c r="H262" s="17"/>
+      <c r="I262" s="17"/>
       <c r="J262" s="1"/>
       <c r="K262" s="1"/>
       <c r="L262" s="1"/>
@@ -9240,15 +9723,21 @@
       <c r="AA262" s="1"/>
     </row>
     <row r="263" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A263" s="17"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
+      <c r="A263" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B263" s="8">
+        <v>43911</v>
+      </c>
+      <c r="C263" s="2">
+        <v>0.27544052621730369</v>
+      </c>
       <c r="D263" s="6"/>
       <c r="E263" s="8"/>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
-      <c r="H263" s="18"/>
-      <c r="I263" s="18"/>
+      <c r="H263" s="17"/>
+      <c r="I263" s="17"/>
       <c r="J263" s="1"/>
       <c r="K263" s="1"/>
       <c r="L263" s="1"/>
@@ -9269,9 +9758,15 @@
       <c r="AA263" s="1"/>
     </row>
     <row r="264" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A264" s="17"/>
-      <c r="B264" s="1"/>
-      <c r="C264" s="19"/>
+      <c r="A264" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B264" s="8">
+        <v>43912</v>
+      </c>
+      <c r="C264" s="21">
+        <v>0.30696204964384161</v>
+      </c>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
       <c r="F264" s="2"/>
@@ -9298,9 +9793,15 @@
       <c r="AA264" s="1"/>
     </row>
     <row r="265" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A265" s="17"/>
-      <c r="B265" s="1"/>
-      <c r="C265" s="19"/>
+      <c r="A265" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B265" s="8">
+        <v>43913</v>
+      </c>
+      <c r="C265" s="21">
+        <v>0.40122092003475646</v>
+      </c>
       <c r="D265" s="1"/>
       <c r="E265" s="1"/>
       <c r="F265" s="2"/>
@@ -9327,9 +9828,15 @@
       <c r="AA265" s="1"/>
     </row>
     <row r="266" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A266" s="17"/>
-      <c r="B266" s="1"/>
-      <c r="C266" s="19"/>
+      <c r="A266" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B266" s="8">
+        <v>43914</v>
+      </c>
+      <c r="C266" s="21">
+        <v>0.79824670912151552</v>
+      </c>
       <c r="D266" s="1"/>
       <c r="E266" s="1"/>
       <c r="F266" s="2"/>
@@ -9356,9 +9863,15 @@
       <c r="AA266" s="1"/>
     </row>
     <row r="267" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A267" s="17"/>
-      <c r="B267" s="1"/>
-      <c r="C267" s="19"/>
+      <c r="A267" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B267" s="8">
+        <v>43915</v>
+      </c>
+      <c r="C267" s="21">
+        <v>0.53261498243103889</v>
+      </c>
       <c r="D267" s="1"/>
       <c r="E267" s="1"/>
       <c r="F267" s="2"/>
@@ -9385,9 +9898,15 @@
       <c r="AA267" s="1"/>
     </row>
     <row r="268" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A268" s="17"/>
-      <c r="B268" s="1"/>
-      <c r="C268" s="19"/>
+      <c r="A268" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B268" s="8">
+        <v>43916</v>
+      </c>
+      <c r="C268" s="21">
+        <v>0.62138312919059635</v>
+      </c>
       <c r="D268" s="1"/>
       <c r="E268" s="1"/>
       <c r="F268" s="2"/>
@@ -9414,9 +9933,15 @@
       <c r="AA268" s="1"/>
     </row>
     <row r="269" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A269" s="17"/>
-      <c r="B269" s="1"/>
-      <c r="C269" s="19"/>
+      <c r="A269" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B269" s="8">
+        <v>43917</v>
+      </c>
+      <c r="C269" s="21">
+        <v>0.77834847176806521</v>
+      </c>
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
       <c r="F269" s="2"/>
@@ -9443,9 +9968,15 @@
       <c r="AA269" s="1"/>
     </row>
     <row r="270" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A270" s="17"/>
-      <c r="B270" s="1"/>
-      <c r="C270" s="19"/>
+      <c r="A270" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B270" s="8">
+        <v>43918</v>
+      </c>
+      <c r="C270" s="21">
+        <v>0.40278433646178341</v>
+      </c>
       <c r="D270" s="1"/>
       <c r="E270" s="1"/>
       <c r="F270" s="2"/>
@@ -9472,9 +10003,15 @@
       <c r="AA270" s="1"/>
     </row>
     <row r="271" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A271" s="17"/>
-      <c r="B271" s="1"/>
-      <c r="C271" s="19"/>
+      <c r="A271" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B271" s="8">
+        <v>43919</v>
+      </c>
+      <c r="C271" s="21">
+        <v>0.23382529426760165</v>
+      </c>
       <c r="D271" s="1"/>
       <c r="E271" s="1"/>
       <c r="F271" s="2"/>
@@ -9501,9 +10038,15 @@
       <c r="AA271" s="1"/>
     </row>
     <row r="272" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A272" s="17"/>
-      <c r="B272" s="1"/>
-      <c r="C272" s="19"/>
+      <c r="A272" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B272" s="8">
+        <v>43920</v>
+      </c>
+      <c r="C272" s="21">
+        <v>0.17698394856866556</v>
+      </c>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
       <c r="F272" s="2"/>
@@ -9530,9 +10073,15 @@
       <c r="AA272" s="1"/>
     </row>
     <row r="273" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A273" s="17"/>
-      <c r="B273" s="1"/>
-      <c r="C273" s="19"/>
+      <c r="A273" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B273" s="8">
+        <v>43921</v>
+      </c>
+      <c r="C273" s="21">
+        <v>0.26022600214366559</v>
+      </c>
       <c r="D273" s="1"/>
       <c r="E273" s="1"/>
       <c r="F273" s="2"/>
@@ -9559,9 +10108,15 @@
       <c r="AA273" s="1"/>
     </row>
     <row r="274" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A274" s="17"/>
-      <c r="B274" s="1"/>
-      <c r="C274" s="19"/>
+      <c r="A274" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B274" s="8">
+        <v>43922</v>
+      </c>
+      <c r="C274" s="21">
+        <v>0.29904432187031033</v>
+      </c>
       <c r="D274" s="1"/>
       <c r="E274" s="1"/>
       <c r="F274" s="2"/>
@@ -9588,9 +10143,15 @@
       <c r="AA274" s="1"/>
     </row>
     <row r="275" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A275" s="17"/>
-      <c r="B275" s="1"/>
-      <c r="C275" s="19"/>
+      <c r="A275" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B275" s="8">
+        <v>43923</v>
+      </c>
+      <c r="C275" s="21">
+        <v>0.38052359030468075</v>
+      </c>
       <c r="D275" s="6"/>
       <c r="E275" s="1"/>
       <c r="F275" s="2"/>
@@ -9617,9 +10178,15 @@
       <c r="AA275" s="1"/>
     </row>
     <row r="276" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A276" s="17"/>
-      <c r="B276" s="1"/>
-      <c r="C276" s="8"/>
+      <c r="A276" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B276" s="8">
+        <v>43924</v>
+      </c>
+      <c r="C276" s="2">
+        <v>0.28694296976580397</v>
+      </c>
       <c r="D276" s="1"/>
       <c r="E276" s="1"/>
       <c r="F276" s="2"/>
@@ -9646,9 +10213,15 @@
       <c r="AA276" s="1"/>
     </row>
     <row r="277" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A277" s="17"/>
-      <c r="B277" s="1"/>
-      <c r="C277" s="8"/>
+      <c r="A277" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B277" s="8">
+        <v>43925</v>
+      </c>
+      <c r="C277" s="2">
+        <v>0.46169803219808442</v>
+      </c>
       <c r="D277" s="1"/>
       <c r="E277" s="1"/>
       <c r="F277" s="2"/>
@@ -9675,9 +10248,15 @@
       <c r="AA277" s="1"/>
     </row>
     <row r="278" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A278" s="17"/>
-      <c r="B278" s="1"/>
-      <c r="C278" s="8"/>
+      <c r="A278" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B278" s="8">
+        <v>43926</v>
+      </c>
+      <c r="C278" s="2">
+        <v>0.98921699681959951</v>
+      </c>
       <c r="D278" s="1"/>
       <c r="E278" s="1"/>
       <c r="F278" s="2"/>
@@ -9704,9 +10283,15 @@
       <c r="AA278" s="1"/>
     </row>
     <row r="279" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A279" s="17"/>
-      <c r="B279" s="1"/>
-      <c r="C279" s="8"/>
+      <c r="A279" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B279" s="8">
+        <v>43927</v>
+      </c>
+      <c r="C279" s="2">
+        <v>0.29246271156331394</v>
+      </c>
       <c r="D279" s="1"/>
       <c r="E279" s="1"/>
       <c r="F279" s="2"/>
@@ -9733,9 +10318,15 @@
       <c r="AA279" s="1"/>
     </row>
     <row r="280" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A280" s="17"/>
-      <c r="B280" s="1"/>
-      <c r="C280" s="8"/>
+      <c r="A280" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B280" s="8">
+        <v>43928</v>
+      </c>
+      <c r="C280" s="2">
+        <v>0.44712753970344182</v>
+      </c>
       <c r="D280" s="1"/>
       <c r="E280" s="1"/>
       <c r="F280" s="2"/>
@@ -9762,9 +10353,15 @@
       <c r="AA280" s="1"/>
     </row>
     <row r="281" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A281" s="17"/>
-      <c r="B281" s="1"/>
-      <c r="C281" s="8"/>
+      <c r="A281" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B281" s="8">
+        <v>43929</v>
+      </c>
+      <c r="C281" s="2">
+        <v>0.55484033510778075</v>
+      </c>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
       <c r="F281" s="2"/>
@@ -9791,9 +10388,15 @@
       <c r="AA281" s="1"/>
     </row>
     <row r="282" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A282" s="17"/>
-      <c r="B282" s="1"/>
-      <c r="C282" s="8"/>
+      <c r="A282" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B282" s="8">
+        <v>43930</v>
+      </c>
+      <c r="C282" s="2">
+        <v>0.52976551720264753</v>
+      </c>
       <c r="D282" s="1"/>
       <c r="E282" s="1"/>
       <c r="F282" s="2"/>
@@ -9820,9 +10423,15 @@
       <c r="AA282" s="1"/>
     </row>
     <row r="283" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A283" s="17"/>
-      <c r="B283" s="1"/>
-      <c r="C283" s="8"/>
+      <c r="A283" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B283" s="8">
+        <v>43931</v>
+      </c>
+      <c r="C283" s="2">
+        <v>0.36037333012705569</v>
+      </c>
       <c r="D283" s="1"/>
       <c r="E283" s="1"/>
       <c r="F283" s="2"/>
@@ -9849,9 +10458,15 @@
       <c r="AA283" s="1"/>
     </row>
     <row r="284" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A284" s="17"/>
-      <c r="B284" s="1"/>
-      <c r="C284" s="8"/>
+      <c r="A284" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B284" s="8">
+        <v>43932</v>
+      </c>
+      <c r="C284" s="2">
+        <v>0.85799276581757378</v>
+      </c>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
       <c r="F284" s="2"/>
@@ -9878,9 +10493,15 @@
       <c r="AA284" s="1"/>
     </row>
     <row r="285" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A285" s="17"/>
-      <c r="B285" s="1"/>
-      <c r="C285" s="8"/>
+      <c r="A285" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B285" s="8">
+        <v>43933</v>
+      </c>
+      <c r="C285" s="2">
+        <v>0.55642005992530041</v>
+      </c>
       <c r="D285" s="1"/>
       <c r="E285" s="1"/>
       <c r="F285" s="2"/>
@@ -9907,9 +10528,15 @@
       <c r="AA285" s="1"/>
     </row>
     <row r="286" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A286" s="17"/>
-      <c r="B286" s="1"/>
-      <c r="C286" s="8"/>
+      <c r="A286" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B286" s="8">
+        <v>43934</v>
+      </c>
+      <c r="C286" s="2">
+        <v>0.36941463951861664</v>
+      </c>
       <c r="D286" s="1"/>
       <c r="E286" s="1"/>
       <c r="F286" s="2"/>
@@ -9936,9 +10563,15 @@
       <c r="AA286" s="1"/>
     </row>
     <row r="287" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A287" s="17"/>
-      <c r="B287" s="1"/>
-      <c r="C287" s="8"/>
+      <c r="A287" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B287" s="8">
+        <v>43935</v>
+      </c>
+      <c r="C287" s="2">
+        <v>0.13054742694596164</v>
+      </c>
       <c r="D287" s="1"/>
       <c r="E287" s="1"/>
       <c r="F287" s="2"/>
@@ -9965,9 +10598,15 @@
       <c r="AA287" s="1"/>
     </row>
     <row r="288" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A288" s="17"/>
-      <c r="B288" s="1"/>
-      <c r="C288" s="8"/>
+      <c r="A288" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B288" s="8">
+        <v>43936</v>
+      </c>
+      <c r="C288" s="2">
+        <v>0.19183919823352555</v>
+      </c>
       <c r="D288" s="1"/>
       <c r="E288" s="1"/>
       <c r="F288" s="2"/>
@@ -9994,9 +10633,15 @@
       <c r="AA288" s="1"/>
     </row>
     <row r="289" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A289" s="17"/>
-      <c r="B289" s="1"/>
-      <c r="C289" s="8"/>
+      <c r="A289" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B289" s="8">
+        <v>43937</v>
+      </c>
+      <c r="C289" s="2">
+        <v>0.24850972413411715</v>
+      </c>
       <c r="D289" s="1"/>
       <c r="E289" s="1"/>
       <c r="F289" s="2"/>
@@ -10023,9 +10668,15 @@
       <c r="AA289" s="1"/>
     </row>
     <row r="290" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A290" s="17"/>
-      <c r="B290" s="1"/>
-      <c r="C290" s="8"/>
+      <c r="A290" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B290" s="8">
+        <v>43938</v>
+      </c>
+      <c r="C290" s="2">
+        <v>0.28102147520128518</v>
+      </c>
       <c r="D290" s="1"/>
       <c r="E290" s="1"/>
       <c r="F290" s="2"/>
@@ -10052,9 +10703,15 @@
       <c r="AA290" s="1"/>
     </row>
     <row r="291" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A291" s="17"/>
-      <c r="B291" s="1"/>
-      <c r="C291" s="8"/>
+      <c r="A291" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B291" s="8">
+        <v>43939</v>
+      </c>
+      <c r="C291" s="2">
+        <v>0.39792748233670805</v>
+      </c>
       <c r="D291" s="1"/>
       <c r="E291" s="1"/>
       <c r="F291" s="2"/>
@@ -10081,9 +10738,15 @@
       <c r="AA291" s="1"/>
     </row>
     <row r="292" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A292" s="17"/>
-      <c r="B292" s="1"/>
-      <c r="C292" s="8"/>
+      <c r="A292" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B292" s="8">
+        <v>43940</v>
+      </c>
+      <c r="C292" s="2">
+        <v>0.3462194310044947</v>
+      </c>
       <c r="D292" s="1"/>
       <c r="E292" s="1"/>
       <c r="F292" s="2"/>
@@ -10110,9 +10773,15 @@
       <c r="AA292" s="1"/>
     </row>
     <row r="293" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A293" s="17"/>
-      <c r="B293" s="1"/>
-      <c r="C293" s="8"/>
+      <c r="A293" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B293" s="8">
+        <v>43941</v>
+      </c>
+      <c r="C293" s="2">
+        <v>0.16371423607702099</v>
+      </c>
       <c r="D293" s="1"/>
       <c r="E293" s="1"/>
       <c r="F293" s="2"/>
@@ -10139,9 +10808,15 @@
       <c r="AA293" s="1"/>
     </row>
     <row r="294" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A294" s="17"/>
-      <c r="B294" s="1"/>
-      <c r="C294" s="8"/>
+      <c r="A294" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B294" s="8">
+        <v>43942</v>
+      </c>
+      <c r="C294" s="2">
+        <v>0.27872217653198439</v>
+      </c>
       <c r="D294" s="6"/>
       <c r="E294" s="1"/>
       <c r="F294" s="2"/>
@@ -10168,9 +10843,15 @@
       <c r="AA294" s="1"/>
     </row>
     <row r="295" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A295" s="1"/>
-      <c r="B295" s="1"/>
-      <c r="C295" s="8"/>
+      <c r="A295" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B295" s="8">
+        <v>43943</v>
+      </c>
+      <c r="C295" s="2">
+        <v>0.23367785580011333</v>
+      </c>
       <c r="D295" s="1"/>
       <c r="E295" s="1"/>
       <c r="F295" s="2"/>
@@ -10197,9 +10878,15 @@
       <c r="AA295" s="1"/>
     </row>
     <row r="296" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A296" s="1"/>
-      <c r="B296" s="1"/>
-      <c r="C296" s="8"/>
+      <c r="A296" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B296" s="8">
+        <v>43944</v>
+      </c>
+      <c r="C296" s="2">
+        <v>0.1907329188831757</v>
+      </c>
       <c r="D296" s="1"/>
       <c r="E296" s="1"/>
       <c r="F296" s="2"/>
@@ -10226,9 +10913,15 @@
       <c r="AA296" s="1"/>
     </row>
     <row r="297" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A297" s="1"/>
-      <c r="B297" s="1"/>
-      <c r="C297" s="8"/>
+      <c r="A297" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B297" s="8">
+        <v>43945</v>
+      </c>
+      <c r="C297" s="2">
+        <v>0.19501064103721194</v>
+      </c>
       <c r="D297" s="1"/>
       <c r="E297" s="1"/>
       <c r="F297" s="2"/>
@@ -10255,9 +10948,15 @@
       <c r="AA297" s="1"/>
     </row>
     <row r="298" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A298" s="1"/>
-      <c r="B298" s="1"/>
-      <c r="C298" s="8"/>
+      <c r="A298" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B298" s="8">
+        <v>43946</v>
+      </c>
+      <c r="C298" s="2">
+        <v>0.16472062786750566</v>
+      </c>
       <c r="D298" s="1"/>
       <c r="E298" s="1"/>
       <c r="F298" s="2"/>
@@ -10284,9 +10983,15 @@
       <c r="AA298" s="1"/>
     </row>
     <row r="299" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A299" s="1"/>
-      <c r="B299" s="1"/>
-      <c r="C299" s="8"/>
+      <c r="A299" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B299" s="8">
+        <v>43947</v>
+      </c>
+      <c r="C299" s="2">
+        <v>0.19171813399747581</v>
+      </c>
       <c r="D299" s="1"/>
       <c r="E299" s="1"/>
       <c r="F299" s="2"/>
@@ -10313,9 +11018,15 @@
       <c r="AA299" s="1"/>
     </row>
     <row r="300" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A300" s="1"/>
-      <c r="B300" s="1"/>
-      <c r="C300" s="8"/>
+      <c r="A300" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B300" s="8">
+        <v>43948</v>
+      </c>
+      <c r="C300" s="2">
+        <v>0.11232798940714318</v>
+      </c>
       <c r="D300" s="1"/>
       <c r="E300" s="1"/>
       <c r="F300" s="2"/>
@@ -10342,9 +11053,15 @@
       <c r="AA300" s="1"/>
     </row>
     <row r="301" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A301" s="1"/>
-      <c r="B301" s="1"/>
-      <c r="C301" s="8"/>
+      <c r="A301" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B301" s="8">
+        <v>43949</v>
+      </c>
+      <c r="C301" s="2">
+        <v>0.34205364906354113</v>
+      </c>
       <c r="D301" s="1"/>
       <c r="E301" s="1"/>
       <c r="F301" s="2"/>
@@ -10371,9 +11088,15 @@
       <c r="AA301" s="1"/>
     </row>
     <row r="302" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A302" s="1"/>
-      <c r="B302" s="1"/>
-      <c r="C302" s="8"/>
+      <c r="A302" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B302" s="8">
+        <v>43950</v>
+      </c>
+      <c r="C302" s="2">
+        <v>0.30615301992876304</v>
+      </c>
       <c r="D302" s="1"/>
       <c r="E302" s="1"/>
       <c r="F302" s="2"/>
@@ -10400,9 +11123,15 @@
       <c r="AA302" s="1"/>
     </row>
     <row r="303" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A303" s="1"/>
-      <c r="B303" s="1"/>
-      <c r="C303" s="8"/>
+      <c r="A303" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B303" s="8">
+        <v>43951</v>
+      </c>
+      <c r="C303" s="2">
+        <v>0.24032506488379621</v>
+      </c>
       <c r="D303" s="1"/>
       <c r="E303" s="1"/>
       <c r="F303" s="2"/>
@@ -10429,9 +11158,15 @@
       <c r="AA303" s="1"/>
     </row>
     <row r="304" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A304" s="1"/>
-      <c r="B304" s="1"/>
-      <c r="C304" s="8"/>
+      <c r="A304" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B304" s="8">
+        <v>43952</v>
+      </c>
+      <c r="C304" s="2">
+        <v>0.1271096702571996</v>
+      </c>
       <c r="D304" s="1"/>
       <c r="E304" s="1"/>
       <c r="F304" s="2"/>
@@ -10458,9 +11193,15 @@
       <c r="AA304" s="1"/>
     </row>
     <row r="305" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A305" s="1"/>
-      <c r="B305" s="1"/>
-      <c r="C305" s="8"/>
+      <c r="A305" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B305" s="8">
+        <v>43953</v>
+      </c>
+      <c r="C305" s="2">
+        <v>0.13933819813510229</v>
+      </c>
       <c r="D305" s="1"/>
       <c r="E305" s="1"/>
       <c r="F305" s="2"/>
@@ -10487,9 +11228,15 @@
       <c r="AA305" s="1"/>
     </row>
     <row r="306" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A306" s="1"/>
-      <c r="B306" s="1"/>
-      <c r="C306" s="8"/>
+      <c r="A306" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B306" s="8">
+        <v>43954</v>
+      </c>
+      <c r="C306" s="2">
+        <v>0.16266141442544566</v>
+      </c>
       <c r="D306" s="1"/>
       <c r="E306" s="1"/>
       <c r="F306" s="2"/>
@@ -10516,9 +11263,15 @@
       <c r="AA306" s="1"/>
     </row>
     <row r="307" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A307" s="1"/>
-      <c r="B307" s="1"/>
-      <c r="C307" s="8"/>
+      <c r="A307" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B307" s="8">
+        <v>43955</v>
+      </c>
+      <c r="C307" s="2">
+        <v>0.38144043036049985</v>
+      </c>
       <c r="D307" s="1"/>
       <c r="E307" s="1"/>
       <c r="F307" s="2"/>
@@ -10545,9 +11298,15 @@
       <c r="AA307" s="1"/>
     </row>
     <row r="308" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A308" s="1"/>
-      <c r="B308" s="1"/>
-      <c r="C308" s="8"/>
+      <c r="A308" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B308" s="8">
+        <v>43956</v>
+      </c>
+      <c r="C308" s="2">
+        <v>0.14466307915285653</v>
+      </c>
       <c r="D308" s="1"/>
       <c r="E308" s="1"/>
       <c r="F308" s="2"/>
@@ -10574,9 +11333,15 @@
       <c r="AA308" s="1"/>
     </row>
     <row r="309" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A309" s="1"/>
-      <c r="B309" s="1"/>
-      <c r="C309" s="8"/>
+      <c r="A309" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B309" s="8">
+        <v>43957</v>
+      </c>
+      <c r="C309" s="2">
+        <v>0.14504167283963593</v>
+      </c>
       <c r="D309" s="1"/>
       <c r="E309" s="1"/>
       <c r="F309" s="2"/>
@@ -10603,9 +11368,15 @@
       <c r="AA309" s="1"/>
     </row>
     <row r="310" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A310" s="1"/>
-      <c r="B310" s="1"/>
-      <c r="C310" s="8"/>
+      <c r="A310" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B310" s="8">
+        <v>43958</v>
+      </c>
+      <c r="C310" s="2">
+        <v>0.19192657561862397</v>
+      </c>
       <c r="D310" s="1"/>
       <c r="E310" s="1"/>
       <c r="F310" s="2"/>
@@ -10632,9 +11403,15 @@
       <c r="AA310" s="1"/>
     </row>
     <row r="311" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A311" s="1"/>
-      <c r="B311" s="1"/>
-      <c r="C311" s="8"/>
+      <c r="A311" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B311" s="8">
+        <v>43959</v>
+      </c>
+      <c r="C311" s="2">
+        <v>0.21596163189246279</v>
+      </c>
       <c r="D311" s="1"/>
       <c r="E311" s="1"/>
       <c r="F311" s="2"/>
@@ -10661,9 +11438,15 @@
       <c r="AA311" s="1"/>
     </row>
     <row r="312" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A312" s="1"/>
-      <c r="B312" s="1"/>
-      <c r="C312" s="8"/>
+      <c r="A312" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B312" s="8">
+        <v>43960</v>
+      </c>
+      <c r="C312" s="2">
+        <v>0.95470458630043809</v>
+      </c>
       <c r="D312" s="1"/>
       <c r="E312" s="1"/>
       <c r="F312" s="2"/>
@@ -10690,9 +11473,15 @@
       <c r="AA312" s="1"/>
     </row>
     <row r="313" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A313" s="1"/>
-      <c r="B313" s="1"/>
-      <c r="C313" s="8"/>
+      <c r="A313" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B313" s="8">
+        <v>43961</v>
+      </c>
+      <c r="C313" s="2">
+        <v>0.48564401916328287</v>
+      </c>
       <c r="D313" s="1"/>
       <c r="E313" s="1"/>
       <c r="F313" s="2"/>
@@ -10719,9 +11508,15 @@
       <c r="AA313" s="1"/>
     </row>
     <row r="314" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A314" s="1"/>
-      <c r="B314" s="1"/>
-      <c r="C314" s="8"/>
+      <c r="A314" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B314" s="8">
+        <v>43962</v>
+      </c>
+      <c r="C314" s="2">
+        <v>0.45607076622761072</v>
+      </c>
       <c r="D314" s="1"/>
       <c r="E314" s="1"/>
       <c r="F314" s="2"/>
@@ -10748,9 +11543,15 @@
       <c r="AA314" s="1"/>
     </row>
     <row r="315" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A315" s="1"/>
-      <c r="B315" s="1"/>
-      <c r="C315" s="8"/>
+      <c r="A315" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B315" s="8">
+        <v>43963</v>
+      </c>
+      <c r="C315" s="2">
+        <v>0.38619222797757358</v>
+      </c>
       <c r="D315" s="1"/>
       <c r="E315" s="1"/>
       <c r="F315" s="2"/>
@@ -10777,9 +11578,15 @@
       <c r="AA315" s="1"/>
     </row>
     <row r="316" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A316" s="1"/>
-      <c r="B316" s="1"/>
-      <c r="C316" s="8"/>
+      <c r="A316" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B316" s="8">
+        <v>43964</v>
+      </c>
+      <c r="C316" s="2">
+        <v>0.18757533701909643</v>
+      </c>
       <c r="D316" s="1"/>
       <c r="E316" s="1"/>
       <c r="F316" s="2"/>
@@ -10806,9 +11613,15 @@
       <c r="AA316" s="1"/>
     </row>
     <row r="317" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A317" s="1"/>
-      <c r="B317" s="1"/>
-      <c r="C317" s="8"/>
+      <c r="A317" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B317" s="8">
+        <v>43965</v>
+      </c>
+      <c r="C317" s="2">
+        <v>0.2467247170979103</v>
+      </c>
       <c r="D317" s="1"/>
       <c r="E317" s="1"/>
       <c r="F317" s="2"/>
@@ -10835,9 +11648,15 @@
       <c r="AA317" s="1"/>
     </row>
     <row r="318" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A318" s="1"/>
-      <c r="B318" s="1"/>
-      <c r="C318" s="8"/>
+      <c r="A318" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B318" s="8">
+        <v>43966</v>
+      </c>
+      <c r="C318" s="2">
+        <v>0.21623088446342009</v>
+      </c>
       <c r="D318" s="1"/>
       <c r="E318" s="1"/>
       <c r="F318" s="2"/>
@@ -10864,9 +11683,15 @@
       <c r="AA318" s="1"/>
     </row>
     <row r="319" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A319" s="1"/>
-      <c r="B319" s="1"/>
-      <c r="C319" s="8"/>
+      <c r="A319" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B319" s="8">
+        <v>43967</v>
+      </c>
+      <c r="C319" s="2">
+        <v>0.31164248361879232</v>
+      </c>
       <c r="D319" s="1"/>
       <c r="E319" s="1"/>
       <c r="F319" s="2"/>
@@ -10893,9 +11718,15 @@
       <c r="AA319" s="1"/>
     </row>
     <row r="320" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A320" s="1"/>
-      <c r="B320" s="1"/>
-      <c r="C320" s="8"/>
+      <c r="A320" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B320" s="8">
+        <v>43968</v>
+      </c>
+      <c r="C320" s="2">
+        <v>0.15350984019578576</v>
+      </c>
       <c r="D320" s="1"/>
       <c r="E320" s="1"/>
       <c r="F320" s="2"/>
@@ -10922,9 +11753,15 @@
       <c r="AA320" s="1"/>
     </row>
     <row r="321" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A321" s="18"/>
-      <c r="B321" s="1"/>
-      <c r="C321" s="20"/>
+      <c r="A321" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B321" s="8">
+        <v>43969</v>
+      </c>
+      <c r="C321" s="19">
+        <v>0.37083291268006313</v>
+      </c>
       <c r="D321" s="1"/>
       <c r="E321" s="1"/>
       <c r="F321" s="2"/>
@@ -10951,9 +11788,15 @@
       <c r="AA321" s="1"/>
     </row>
     <row r="322" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A322" s="18"/>
-      <c r="B322" s="1"/>
-      <c r="C322" s="20"/>
+      <c r="A322" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B322" s="8">
+        <v>43970</v>
+      </c>
+      <c r="C322" s="19">
+        <v>0.1554394139606054</v>
+      </c>
       <c r="D322" s="1"/>
       <c r="E322" s="1"/>
       <c r="F322" s="2"/>
@@ -10980,9 +11823,15 @@
       <c r="AA322" s="1"/>
     </row>
     <row r="323" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A323" s="18"/>
-      <c r="B323" s="1"/>
-      <c r="C323" s="20"/>
+      <c r="A323" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B323" s="8">
+        <v>43971</v>
+      </c>
+      <c r="C323" s="19">
+        <v>0.50819085152919652</v>
+      </c>
       <c r="D323" s="1"/>
       <c r="E323" s="1"/>
       <c r="F323" s="2"/>
@@ -11009,9 +11858,15 @@
       <c r="AA323" s="1"/>
     </row>
     <row r="324" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A324" s="18"/>
-      <c r="B324" s="1"/>
-      <c r="C324" s="20"/>
+      <c r="A324" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B324" s="8">
+        <v>43972</v>
+      </c>
+      <c r="C324" s="19">
+        <v>0.97926335816194932</v>
+      </c>
       <c r="D324" s="1"/>
       <c r="E324" s="1"/>
       <c r="F324" s="2"/>
@@ -11038,9 +11893,15 @@
       <c r="AA324" s="1"/>
     </row>
     <row r="325" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A325" s="18"/>
-      <c r="B325" s="1"/>
-      <c r="C325" s="20"/>
+      <c r="A325" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B325" s="8">
+        <v>43973</v>
+      </c>
+      <c r="C325" s="19">
+        <v>0.96707970332129289</v>
+      </c>
       <c r="D325" s="1"/>
       <c r="E325" s="1"/>
       <c r="F325" s="2"/>
@@ -11067,9 +11928,15 @@
       <c r="AA325" s="1"/>
     </row>
     <row r="326" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A326" s="18"/>
-      <c r="B326" s="1"/>
-      <c r="C326" s="20"/>
+      <c r="A326" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B326" s="8">
+        <v>43974</v>
+      </c>
+      <c r="C326" s="19">
+        <v>0.85579504577009513</v>
+      </c>
       <c r="D326" s="1"/>
       <c r="E326" s="1"/>
       <c r="F326" s="2"/>
@@ -11096,9 +11963,15 @@
       <c r="AA326" s="1"/>
     </row>
     <row r="327" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A327" s="18"/>
-      <c r="B327" s="1"/>
-      <c r="C327" s="20"/>
+      <c r="A327" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B327" s="8">
+        <v>43975</v>
+      </c>
+      <c r="C327" s="19">
+        <v>0.15999669642445113</v>
+      </c>
       <c r="D327" s="6"/>
       <c r="E327" s="1"/>
       <c r="F327" s="2"/>
@@ -11125,9 +11998,15 @@
       <c r="AA327" s="1"/>
     </row>
     <row r="328" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A328" s="18"/>
-      <c r="B328" s="1"/>
-      <c r="C328" s="20"/>
+      <c r="A328" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B328" s="8">
+        <v>43976</v>
+      </c>
+      <c r="C328" s="19">
+        <v>0.11764904838159539</v>
+      </c>
       <c r="D328" s="1"/>
       <c r="E328" s="1"/>
       <c r="F328" s="2"/>
@@ -11154,9 +12033,15 @@
       <c r="AA328" s="1"/>
     </row>
     <row r="329" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A329" s="18"/>
-      <c r="B329" s="1"/>
-      <c r="C329" s="20"/>
+      <c r="A329" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B329" s="8">
+        <v>43977</v>
+      </c>
+      <c r="C329" s="19">
+        <v>0.22767180825726052</v>
+      </c>
       <c r="D329" s="1"/>
       <c r="E329" s="1"/>
       <c r="F329" s="2"/>
@@ -11183,9 +12068,15 @@
       <c r="AA329" s="1"/>
     </row>
     <row r="330" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A330" s="18"/>
-      <c r="B330" s="1"/>
-      <c r="C330" s="20"/>
+      <c r="A330" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B330" s="8">
+        <v>43978</v>
+      </c>
+      <c r="C330" s="19">
+        <v>0.20702937438922503</v>
+      </c>
       <c r="D330" s="1"/>
       <c r="E330" s="1"/>
       <c r="F330" s="2"/>
@@ -11212,9 +12103,15 @@
       <c r="AA330" s="1"/>
     </row>
     <row r="331" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A331" s="18"/>
-      <c r="B331" s="1"/>
-      <c r="C331" s="20"/>
+      <c r="A331" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B331" s="8">
+        <v>43979</v>
+      </c>
+      <c r="C331" s="19">
+        <v>0.17807160403336822</v>
+      </c>
       <c r="D331" s="1"/>
       <c r="E331" s="1"/>
       <c r="F331" s="2"/>
@@ -11241,9 +12138,15 @@
       <c r="AA331" s="1"/>
     </row>
     <row r="332" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A332" s="18"/>
-      <c r="B332" s="1"/>
-      <c r="C332" s="20"/>
+      <c r="A332" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B332" s="8">
+        <v>43980</v>
+      </c>
+      <c r="C332" s="19">
+        <v>0.18132065839838882</v>
+      </c>
       <c r="D332" s="1"/>
       <c r="E332" s="1"/>
       <c r="F332" s="2"/>
@@ -11270,9 +12173,15 @@
       <c r="AA332" s="1"/>
     </row>
     <row r="333" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A333" s="18"/>
-      <c r="B333" s="1"/>
-      <c r="C333" s="20"/>
+      <c r="A333" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B333" s="8">
+        <v>43981</v>
+      </c>
+      <c r="C333" s="19">
+        <v>0.15043863303740543</v>
+      </c>
       <c r="D333" s="1"/>
       <c r="E333" s="1"/>
       <c r="F333" s="2"/>
@@ -11299,9 +12208,15 @@
       <c r="AA333" s="1"/>
     </row>
     <row r="334" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A334" s="18"/>
-      <c r="B334" s="1"/>
-      <c r="C334" s="20"/>
+      <c r="A334" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B334" s="8">
+        <v>43982</v>
+      </c>
+      <c r="C334" s="19">
+        <v>0.12801626394462842</v>
+      </c>
       <c r="D334" s="6"/>
       <c r="E334" s="1"/>
       <c r="F334" s="2"/>
@@ -11328,9 +12243,15 @@
       <c r="AA334" s="1"/>
     </row>
     <row r="335" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A335" s="18"/>
-      <c r="B335" s="1"/>
-      <c r="C335" s="20"/>
+      <c r="A335" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B335" s="8">
+        <v>43983</v>
+      </c>
+      <c r="C335" s="19">
+        <v>0.13800627741411528</v>
+      </c>
       <c r="D335" s="1"/>
       <c r="E335" s="1"/>
       <c r="F335" s="2"/>
@@ -11357,9 +12278,15 @@
       <c r="AA335" s="1"/>
     </row>
     <row r="336" spans="1:27" x14ac:dyDescent="0.5">
-      <c r="A336" s="18"/>
-      <c r="B336" s="1"/>
-      <c r="C336" s="20"/>
+      <c r="A336" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B336" s="8">
+        <v>43984</v>
+      </c>
+      <c r="C336" s="19">
+        <v>0.13231283945782799</v>
+      </c>
       <c r="D336" s="1"/>
       <c r="E336" s="1"/>
       <c r="F336" s="2"/>
@@ -11386,9 +12313,15 @@
       <c r="AA336" s="1"/>
     </row>
     <row r="337" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A337" s="18"/>
-      <c r="B337" s="1"/>
-      <c r="C337" s="20"/>
+      <c r="A337" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B337" s="8">
+        <v>43985</v>
+      </c>
+      <c r="C337" s="19">
+        <v>0.1194082558533115</v>
+      </c>
       <c r="D337" s="1"/>
       <c r="E337" s="1"/>
       <c r="F337" s="2"/>
@@ -11415,9 +12348,15 @@
       <c r="AA337" s="1"/>
     </row>
     <row r="338" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A338" s="18"/>
-      <c r="B338" s="1"/>
-      <c r="C338" s="20"/>
+      <c r="A338" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B338" s="8">
+        <v>43986</v>
+      </c>
+      <c r="C338" s="19">
+        <v>0.16149628784517653</v>
+      </c>
       <c r="D338" s="1"/>
       <c r="E338" s="1"/>
       <c r="F338" s="2"/>
@@ -11444,9 +12383,15 @@
       <c r="AA338" s="1"/>
     </row>
     <row r="339" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A339" s="18"/>
-      <c r="B339" s="1"/>
-      <c r="C339" s="20"/>
+      <c r="A339" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B339" s="8">
+        <v>43987</v>
+      </c>
+      <c r="C339" s="19">
+        <v>0.16349690155290705</v>
+      </c>
       <c r="D339" s="1"/>
       <c r="E339" s="1"/>
       <c r="F339" s="2"/>
@@ -11473,9 +12418,15 @@
       <c r="AA339" s="1"/>
     </row>
     <row r="340" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A340" s="18"/>
-      <c r="B340" s="1"/>
-      <c r="C340" s="20"/>
+      <c r="A340" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B340" s="8">
+        <v>43988</v>
+      </c>
+      <c r="C340" s="19">
+        <v>0.22430112737379229</v>
+      </c>
       <c r="D340" s="6"/>
       <c r="E340" s="1"/>
       <c r="F340" s="2"/>
@@ -11502,9 +12453,15 @@
       <c r="AA340" s="1"/>
     </row>
     <row r="341" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A341" s="18"/>
-      <c r="B341" s="1"/>
-      <c r="C341" s="20"/>
+      <c r="A341" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B341" s="8">
+        <v>43989</v>
+      </c>
+      <c r="C341" s="19">
+        <v>0.22838171258307866</v>
+      </c>
       <c r="D341" s="1"/>
       <c r="E341" s="1"/>
       <c r="F341" s="2"/>
@@ -11526,16 +12483,22 @@
       <c r="V341" s="2"/>
       <c r="W341" s="2"/>
       <c r="X341" s="2"/>
-      <c r="Y341" s="21"/>
+      <c r="Y341" s="19"/>
       <c r="Z341" s="2"/>
       <c r="AA341" s="2"/>
       <c r="AB341" s="7"/>
       <c r="AC341" s="7"/>
     </row>
     <row r="342" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A342" s="18"/>
-      <c r="B342" s="1"/>
-      <c r="C342" s="20"/>
+      <c r="A342" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B342" s="8">
+        <v>43990</v>
+      </c>
+      <c r="C342" s="19">
+        <v>0.21485270202767642</v>
+      </c>
       <c r="D342" s="1"/>
       <c r="E342" s="1"/>
       <c r="F342" s="2"/>
@@ -11557,16 +12520,22 @@
       <c r="V342" s="2"/>
       <c r="W342" s="2"/>
       <c r="X342" s="2"/>
-      <c r="Y342" s="21"/>
+      <c r="Y342" s="19"/>
       <c r="Z342" s="2"/>
       <c r="AA342" s="2"/>
       <c r="AB342" s="7"/>
       <c r="AC342" s="7"/>
     </row>
     <row r="343" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A343" s="18"/>
-      <c r="B343" s="1"/>
-      <c r="C343" s="20"/>
+      <c r="A343" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B343" s="8">
+        <v>43991</v>
+      </c>
+      <c r="C343" s="19">
+        <v>0.32536585980822613</v>
+      </c>
       <c r="D343" s="1"/>
       <c r="E343" s="1"/>
       <c r="F343" s="2"/>
@@ -11583,21 +12552,27 @@
       <c r="Q343" s="2"/>
       <c r="R343" s="2"/>
       <c r="S343" s="2"/>
-      <c r="T343" s="21"/>
+      <c r="T343" s="19"/>
       <c r="U343" s="2"/>
       <c r="V343" s="2"/>
       <c r="W343" s="2"/>
       <c r="X343" s="2"/>
-      <c r="Y343" s="21"/>
+      <c r="Y343" s="19"/>
       <c r="Z343" s="2"/>
       <c r="AA343" s="2"/>
       <c r="AB343" s="7"/>
       <c r="AC343" s="7"/>
     </row>
     <row r="344" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A344" s="18"/>
-      <c r="B344" s="1"/>
-      <c r="C344" s="20"/>
+      <c r="A344" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B344" s="8">
+        <v>43992</v>
+      </c>
+      <c r="C344" s="19">
+        <v>0.23773168777702364</v>
+      </c>
       <c r="D344" s="1"/>
       <c r="E344" s="1"/>
       <c r="F344" s="2"/>
@@ -11614,21 +12589,27 @@
       <c r="Q344" s="2"/>
       <c r="R344" s="2"/>
       <c r="S344" s="2"/>
-      <c r="T344" s="21"/>
+      <c r="T344" s="19"/>
       <c r="U344" s="2"/>
       <c r="V344" s="2"/>
       <c r="W344" s="2"/>
       <c r="X344" s="2"/>
-      <c r="Y344" s="21"/>
+      <c r="Y344" s="19"/>
       <c r="Z344" s="2"/>
       <c r="AA344" s="2"/>
       <c r="AB344" s="7"/>
       <c r="AC344" s="7"/>
     </row>
     <row r="345" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A345" s="18"/>
-      <c r="B345" s="1"/>
-      <c r="C345" s="20"/>
+      <c r="A345" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B345" s="8">
+        <v>43993</v>
+      </c>
+      <c r="C345" s="19">
+        <v>0.35381781003775015</v>
+      </c>
       <c r="D345" s="1"/>
       <c r="E345" s="1"/>
       <c r="F345" s="2"/>
@@ -11650,16 +12631,22 @@
       <c r="V345" s="2"/>
       <c r="W345" s="2"/>
       <c r="X345" s="2"/>
-      <c r="Y345" s="21"/>
+      <c r="Y345" s="19"/>
       <c r="Z345" s="2"/>
       <c r="AA345" s="2"/>
       <c r="AB345" s="7"/>
       <c r="AC345" s="7"/>
     </row>
     <row r="346" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A346" s="18"/>
-      <c r="B346" s="1"/>
-      <c r="C346" s="20"/>
+      <c r="A346" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B346" s="8">
+        <v>43994</v>
+      </c>
+      <c r="C346" s="19">
+        <v>0.20251615557568392</v>
+      </c>
       <c r="D346" s="6"/>
       <c r="E346" s="1"/>
       <c r="F346" s="2"/>
@@ -11676,21 +12663,27 @@
       <c r="Q346" s="2"/>
       <c r="R346" s="2"/>
       <c r="S346" s="2"/>
-      <c r="T346" s="21"/>
+      <c r="T346" s="19"/>
       <c r="U346" s="2"/>
       <c r="V346" s="2"/>
       <c r="W346" s="2"/>
       <c r="X346" s="2"/>
-      <c r="Y346" s="21"/>
+      <c r="Y346" s="19"/>
       <c r="Z346" s="2"/>
       <c r="AA346" s="2"/>
       <c r="AB346" s="7"/>
       <c r="AC346" s="7"/>
     </row>
     <row r="347" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A347" s="18"/>
-      <c r="B347" s="1"/>
-      <c r="C347" s="20"/>
+      <c r="A347" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B347" s="8">
+        <v>43995</v>
+      </c>
+      <c r="C347" s="19">
+        <v>0.18189728571354846</v>
+      </c>
       <c r="D347" s="1"/>
       <c r="E347" s="1"/>
       <c r="F347" s="2"/>
@@ -11712,16 +12705,22 @@
       <c r="V347" s="2"/>
       <c r="W347" s="2"/>
       <c r="X347" s="2"/>
-      <c r="Y347" s="21"/>
+      <c r="Y347" s="19"/>
       <c r="Z347" s="2"/>
       <c r="AA347" s="2"/>
       <c r="AB347" s="7"/>
       <c r="AC347" s="7"/>
     </row>
     <row r="348" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A348" s="18"/>
-      <c r="B348" s="1"/>
-      <c r="C348" s="20"/>
+      <c r="A348" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B348" s="8">
+        <v>43996</v>
+      </c>
+      <c r="C348" s="19">
+        <v>0.12630748908405504</v>
+      </c>
       <c r="D348" s="1"/>
       <c r="E348" s="1"/>
       <c r="F348" s="2"/>
@@ -11743,16 +12742,22 @@
       <c r="V348" s="2"/>
       <c r="W348" s="2"/>
       <c r="X348" s="2"/>
-      <c r="Y348" s="21"/>
+      <c r="Y348" s="19"/>
       <c r="Z348" s="2"/>
       <c r="AA348" s="2"/>
       <c r="AB348" s="7"/>
       <c r="AC348" s="7"/>
     </row>
     <row r="349" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A349" s="18"/>
-      <c r="B349" s="1"/>
-      <c r="C349" s="20"/>
+      <c r="A349" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B349" s="8">
+        <v>43997</v>
+      </c>
+      <c r="C349" s="19">
+        <v>0.15664383967645612</v>
+      </c>
       <c r="D349" s="1"/>
       <c r="E349" s="1"/>
       <c r="F349" s="2"/>
@@ -11769,21 +12774,27 @@
       <c r="Q349" s="2"/>
       <c r="R349" s="2"/>
       <c r="S349" s="2"/>
-      <c r="T349" s="21"/>
+      <c r="T349" s="19"/>
       <c r="U349" s="2"/>
       <c r="V349" s="2"/>
       <c r="W349" s="2"/>
       <c r="X349" s="2"/>
-      <c r="Y349" s="21"/>
+      <c r="Y349" s="19"/>
       <c r="Z349" s="2"/>
       <c r="AA349" s="2"/>
       <c r="AB349" s="7"/>
       <c r="AC349" s="7"/>
     </row>
     <row r="350" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A350" s="18"/>
-      <c r="B350" s="1"/>
-      <c r="C350" s="20"/>
+      <c r="A350" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B350" s="8">
+        <v>43998</v>
+      </c>
+      <c r="C350" s="19">
+        <v>0.27419109401868741</v>
+      </c>
       <c r="D350" s="1"/>
       <c r="E350" s="1"/>
       <c r="F350" s="2"/>
@@ -11800,21 +12811,27 @@
       <c r="Q350" s="2"/>
       <c r="R350" s="2"/>
       <c r="S350" s="2"/>
-      <c r="T350" s="21"/>
+      <c r="T350" s="19"/>
       <c r="U350" s="2"/>
       <c r="V350" s="2"/>
       <c r="W350" s="2"/>
       <c r="X350" s="2"/>
-      <c r="Y350" s="21"/>
+      <c r="Y350" s="19"/>
       <c r="Z350" s="2"/>
       <c r="AA350" s="2"/>
       <c r="AB350" s="7"/>
       <c r="AC350" s="7"/>
     </row>
     <row r="351" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A351" s="18"/>
-      <c r="B351" s="1"/>
-      <c r="C351" s="20"/>
+      <c r="A351" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B351" s="8">
+        <v>43999</v>
+      </c>
+      <c r="C351" s="19">
+        <v>0.1332312275851073</v>
+      </c>
       <c r="D351" s="1"/>
       <c r="E351" s="1"/>
       <c r="F351" s="2"/>
@@ -11831,21 +12848,27 @@
       <c r="Q351" s="2"/>
       <c r="R351" s="2"/>
       <c r="S351" s="2"/>
-      <c r="T351" s="21"/>
+      <c r="T351" s="19"/>
       <c r="U351" s="2"/>
       <c r="V351" s="2"/>
       <c r="W351" s="2"/>
       <c r="X351" s="2"/>
-      <c r="Y351" s="21"/>
+      <c r="Y351" s="19"/>
       <c r="Z351" s="2"/>
       <c r="AA351" s="2"/>
       <c r="AB351" s="7"/>
       <c r="AC351" s="7"/>
     </row>
     <row r="352" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A352" s="18"/>
-      <c r="B352" s="1"/>
-      <c r="C352" s="20"/>
+      <c r="A352" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B352" s="8">
+        <v>44000</v>
+      </c>
+      <c r="C352" s="19">
+        <v>0.16169845734594498</v>
+      </c>
       <c r="D352" s="6"/>
       <c r="E352" s="1"/>
       <c r="F352" s="2"/>
@@ -11862,21 +12885,27 @@
       <c r="Q352" s="2"/>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
-      <c r="T352" s="21"/>
+      <c r="T352" s="19"/>
       <c r="U352" s="2"/>
       <c r="V352" s="2"/>
       <c r="W352" s="2"/>
       <c r="X352" s="2"/>
-      <c r="Y352" s="21"/>
+      <c r="Y352" s="19"/>
       <c r="Z352" s="2"/>
       <c r="AA352" s="2"/>
       <c r="AB352" s="7"/>
       <c r="AC352" s="7"/>
     </row>
     <row r="353" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A353" s="18"/>
-      <c r="B353" s="1"/>
-      <c r="C353" s="20"/>
+      <c r="A353" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B353" s="8">
+        <v>44001</v>
+      </c>
+      <c r="C353" s="19">
+        <v>0.14432273798106138</v>
+      </c>
       <c r="D353" s="1"/>
       <c r="E353" s="1"/>
       <c r="F353" s="2"/>
@@ -11898,16 +12927,22 @@
       <c r="V353" s="2"/>
       <c r="W353" s="2"/>
       <c r="X353" s="2"/>
-      <c r="Y353" s="21"/>
+      <c r="Y353" s="19"/>
       <c r="Z353" s="2"/>
       <c r="AA353" s="2"/>
       <c r="AB353" s="7"/>
       <c r="AC353" s="7"/>
     </row>
     <row r="354" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A354" s="18"/>
-      <c r="B354" s="1"/>
-      <c r="C354" s="20"/>
+      <c r="A354" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B354" s="8">
+        <v>44002</v>
+      </c>
+      <c r="C354" s="19">
+        <v>0.20711780804999677</v>
+      </c>
       <c r="D354" s="1"/>
       <c r="E354" s="1"/>
       <c r="F354" s="2"/>
@@ -11929,16 +12964,22 @@
       <c r="V354" s="2"/>
       <c r="W354" s="2"/>
       <c r="X354" s="2"/>
-      <c r="Y354" s="21"/>
+      <c r="Y354" s="19"/>
       <c r="Z354" s="2"/>
       <c r="AA354" s="2"/>
       <c r="AB354" s="7"/>
       <c r="AC354" s="7"/>
     </row>
     <row r="355" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A355" s="18"/>
-      <c r="B355" s="1"/>
-      <c r="C355" s="20"/>
+      <c r="A355" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B355" s="8">
+        <v>44003</v>
+      </c>
+      <c r="C355" s="19">
+        <v>0.1545301924301907</v>
+      </c>
       <c r="D355" s="1"/>
       <c r="E355" s="1"/>
       <c r="F355" s="2"/>
@@ -11955,21 +12996,27 @@
       <c r="Q355" s="2"/>
       <c r="R355" s="2"/>
       <c r="S355" s="2"/>
-      <c r="T355" s="21"/>
+      <c r="T355" s="19"/>
       <c r="U355" s="2"/>
       <c r="V355" s="2"/>
       <c r="W355" s="2"/>
       <c r="X355" s="2"/>
-      <c r="Y355" s="21"/>
+      <c r="Y355" s="19"/>
       <c r="Z355" s="2"/>
       <c r="AA355" s="2"/>
       <c r="AB355" s="7"/>
       <c r="AC355" s="7"/>
     </row>
     <row r="356" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A356" s="18"/>
-      <c r="B356" s="1"/>
-      <c r="C356" s="20"/>
+      <c r="A356" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B356" s="8">
+        <v>44004</v>
+      </c>
+      <c r="C356" s="19">
+        <v>0.15957057412195624</v>
+      </c>
       <c r="D356" s="1"/>
       <c r="E356" s="1"/>
       <c r="F356" s="2"/>
@@ -11986,21 +13033,27 @@
       <c r="Q356" s="2"/>
       <c r="R356" s="2"/>
       <c r="S356" s="2"/>
-      <c r="T356" s="21"/>
+      <c r="T356" s="19"/>
       <c r="U356" s="2"/>
       <c r="V356" s="2"/>
       <c r="W356" s="2"/>
       <c r="X356" s="2"/>
-      <c r="Y356" s="21"/>
+      <c r="Y356" s="19"/>
       <c r="Z356" s="2"/>
       <c r="AA356" s="2"/>
       <c r="AB356" s="7"/>
       <c r="AC356" s="7"/>
     </row>
     <row r="357" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A357" s="18"/>
-      <c r="B357" s="1"/>
-      <c r="C357" s="20"/>
+      <c r="A357" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B357" s="8">
+        <v>44005</v>
+      </c>
+      <c r="C357" s="19">
+        <v>0.15917492961194732</v>
+      </c>
       <c r="D357" s="1"/>
       <c r="E357" s="1"/>
       <c r="F357" s="2"/>
@@ -12017,21 +13070,27 @@
       <c r="Q357" s="2"/>
       <c r="R357" s="2"/>
       <c r="S357" s="2"/>
-      <c r="T357" s="21"/>
+      <c r="T357" s="19"/>
       <c r="U357" s="2"/>
       <c r="V357" s="2"/>
       <c r="W357" s="2"/>
       <c r="X357" s="2"/>
-      <c r="Y357" s="21"/>
+      <c r="Y357" s="19"/>
       <c r="Z357" s="2"/>
       <c r="AA357" s="2"/>
       <c r="AB357" s="7"/>
       <c r="AC357" s="7"/>
     </row>
     <row r="358" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A358" s="18"/>
-      <c r="B358" s="1"/>
-      <c r="C358" s="20"/>
+      <c r="A358" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B358" s="8">
+        <v>44006</v>
+      </c>
+      <c r="C358" s="19">
+        <v>0.19053888194921231</v>
+      </c>
       <c r="D358" s="6"/>
       <c r="E358" s="1"/>
       <c r="F358" s="2"/>
@@ -12048,21 +13107,27 @@
       <c r="Q358" s="2"/>
       <c r="R358" s="2"/>
       <c r="S358" s="2"/>
-      <c r="T358" s="21"/>
+      <c r="T358" s="19"/>
       <c r="U358" s="2"/>
       <c r="V358" s="2"/>
       <c r="W358" s="2"/>
       <c r="X358" s="2"/>
-      <c r="Y358" s="21"/>
+      <c r="Y358" s="19"/>
       <c r="Z358" s="2"/>
       <c r="AA358" s="2"/>
       <c r="AB358" s="7"/>
       <c r="AC358" s="7"/>
     </row>
     <row r="359" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A359" s="18"/>
-      <c r="B359" s="1"/>
-      <c r="C359" s="20"/>
+      <c r="A359" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B359" s="8">
+        <v>44007</v>
+      </c>
+      <c r="C359" s="19">
+        <v>0.1709967775265942</v>
+      </c>
       <c r="D359" s="1"/>
       <c r="E359" s="1"/>
       <c r="F359" s="2"/>
@@ -12084,16 +13149,22 @@
       <c r="V359" s="2"/>
       <c r="W359" s="2"/>
       <c r="X359" s="2"/>
-      <c r="Y359" s="21"/>
+      <c r="Y359" s="19"/>
       <c r="Z359" s="2"/>
       <c r="AA359" s="2"/>
       <c r="AB359" s="7"/>
       <c r="AC359" s="7"/>
     </row>
     <row r="360" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A360" s="18"/>
-      <c r="B360" s="1"/>
-      <c r="C360" s="20"/>
+      <c r="A360" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B360" s="8">
+        <v>44008</v>
+      </c>
+      <c r="C360" s="19">
+        <v>0.15193171470159281</v>
+      </c>
       <c r="D360" s="1"/>
       <c r="E360" s="1"/>
       <c r="F360" s="2"/>
@@ -12115,16 +13186,22 @@
       <c r="V360" s="2"/>
       <c r="W360" s="2"/>
       <c r="X360" s="2"/>
-      <c r="Y360" s="21"/>
+      <c r="Y360" s="19"/>
       <c r="Z360" s="2"/>
       <c r="AA360" s="2"/>
       <c r="AB360" s="7"/>
       <c r="AC360" s="7"/>
     </row>
     <row r="361" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A361" s="18"/>
-      <c r="B361" s="1"/>
-      <c r="C361" s="20"/>
+      <c r="A361" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B361" s="8">
+        <v>44009</v>
+      </c>
+      <c r="C361" s="19">
+        <v>0.1865661198641772</v>
+      </c>
       <c r="D361" s="1"/>
       <c r="E361" s="1"/>
       <c r="F361" s="2"/>
@@ -12141,21 +13218,27 @@
       <c r="Q361" s="2"/>
       <c r="R361" s="2"/>
       <c r="S361" s="2"/>
-      <c r="T361" s="21"/>
+      <c r="T361" s="19"/>
       <c r="U361" s="2"/>
       <c r="V361" s="2"/>
       <c r="W361" s="2"/>
       <c r="X361" s="2"/>
-      <c r="Y361" s="21"/>
+      <c r="Y361" s="19"/>
       <c r="Z361" s="2"/>
       <c r="AA361" s="2"/>
       <c r="AB361" s="7"/>
       <c r="AC361" s="7"/>
     </row>
     <row r="362" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A362" s="18"/>
-      <c r="B362" s="1"/>
-      <c r="C362" s="20"/>
+      <c r="A362" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B362" s="8">
+        <v>44010</v>
+      </c>
+      <c r="C362" s="19">
+        <v>0.14406344167150847</v>
+      </c>
       <c r="D362" s="1"/>
       <c r="E362" s="1"/>
       <c r="F362" s="2"/>
@@ -12172,21 +13255,27 @@
       <c r="Q362" s="2"/>
       <c r="R362" s="2"/>
       <c r="S362" s="2"/>
-      <c r="T362" s="21"/>
+      <c r="T362" s="19"/>
       <c r="U362" s="2"/>
       <c r="V362" s="2"/>
       <c r="W362" s="2"/>
       <c r="X362" s="2"/>
-      <c r="Y362" s="21"/>
+      <c r="Y362" s="19"/>
       <c r="Z362" s="2"/>
       <c r="AA362" s="2"/>
       <c r="AB362" s="7"/>
       <c r="AC362" s="7"/>
     </row>
     <row r="363" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A363" s="18"/>
-      <c r="B363" s="1"/>
-      <c r="C363" s="20"/>
+      <c r="A363" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B363" s="8">
+        <v>44011</v>
+      </c>
+      <c r="C363" s="19">
+        <v>0.294939130550043</v>
+      </c>
       <c r="D363" s="1"/>
       <c r="E363" s="1"/>
       <c r="F363" s="2"/>
@@ -12203,21 +13292,21 @@
       <c r="Q363" s="2"/>
       <c r="R363" s="2"/>
       <c r="S363" s="2"/>
-      <c r="T363" s="21"/>
+      <c r="T363" s="19"/>
       <c r="U363" s="2"/>
       <c r="V363" s="2"/>
       <c r="W363" s="2"/>
       <c r="X363" s="2"/>
-      <c r="Y363" s="21"/>
+      <c r="Y363" s="19"/>
       <c r="Z363" s="2"/>
       <c r="AA363" s="2"/>
       <c r="AB363" s="7"/>
       <c r="AC363" s="7"/>
     </row>
     <row r="364" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A364" s="18"/>
+      <c r="A364" s="17"/>
       <c r="B364" s="1"/>
-      <c r="C364" s="20"/>
+      <c r="C364" s="18"/>
       <c r="D364" s="6"/>
       <c r="E364" s="1"/>
       <c r="F364" s="2"/>
@@ -12234,12 +13323,12 @@
       <c r="Q364" s="2"/>
       <c r="R364" s="2"/>
       <c r="S364" s="2"/>
-      <c r="T364" s="21"/>
+      <c r="T364" s="19"/>
       <c r="U364" s="2"/>
       <c r="V364" s="2"/>
       <c r="W364" s="2"/>
       <c r="X364" s="2"/>
-      <c r="Y364" s="21"/>
+      <c r="Y364" s="19"/>
       <c r="Z364" s="2"/>
       <c r="AA364" s="2"/>
       <c r="AB364" s="7"/>

</xml_diff>

<commit_message>
Add test for Arid locations
</commit_message>
<xml_diff>
--- a/Tests/Validation/Weather/Observed.xlsx
+++ b/Tests/Validation/Weather/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\Weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F16C38-A566-40A1-AD27-004DBA9CA254}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1718B308-B615-47C2-A746-480AF991FFB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="6">
   <si>
     <t>SimulationName</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>DarwinRadiation</t>
+  </si>
+  <si>
+    <t>AliceSpringsRadiation</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -148,7 +151,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -536,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE028B48-E928-4E9E-80FD-208C4FFEA9B6}">
-  <dimension ref="A1:AC364"/>
+  <dimension ref="A1:AC544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183:C363"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="C364" sqref="C364:C544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -6926,7 +6928,7 @@
       <c r="A183" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B183" s="20">
+      <c r="B183" s="19">
         <v>43831</v>
       </c>
       <c r="C183" s="7">
@@ -6961,7 +6963,7 @@
       <c r="A184" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B184" s="20">
+      <c r="B184" s="19">
         <v>43832</v>
       </c>
       <c r="C184" s="7">
@@ -6996,7 +6998,7 @@
       <c r="A185" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B185" s="20">
+      <c r="B185" s="19">
         <v>43833</v>
       </c>
       <c r="C185" s="7">
@@ -7031,7 +7033,7 @@
       <c r="A186" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B186" s="20">
+      <c r="B186" s="19">
         <v>43834</v>
       </c>
       <c r="C186" s="7">
@@ -7066,7 +7068,7 @@
       <c r="A187" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B187" s="20">
+      <c r="B187" s="19">
         <v>43835</v>
       </c>
       <c r="C187" s="7">
@@ -7101,7 +7103,7 @@
       <c r="A188" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B188" s="20">
+      <c r="B188" s="19">
         <v>43836</v>
       </c>
       <c r="C188" s="7">
@@ -7136,7 +7138,7 @@
       <c r="A189" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B189" s="20">
+      <c r="B189" s="19">
         <v>43837</v>
       </c>
       <c r="C189" s="7">
@@ -7171,7 +7173,7 @@
       <c r="A190" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B190" s="20">
+      <c r="B190" s="19">
         <v>43838</v>
       </c>
       <c r="C190" s="12">
@@ -7206,7 +7208,7 @@
       <c r="A191" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B191" s="20">
+      <c r="B191" s="19">
         <v>43839</v>
       </c>
       <c r="C191" s="12">
@@ -7241,7 +7243,7 @@
       <c r="A192" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B192" s="20">
+      <c r="B192" s="19">
         <v>43840</v>
       </c>
       <c r="C192" s="12">
@@ -7276,7 +7278,7 @@
       <c r="A193" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B193" s="20">
+      <c r="B193" s="19">
         <v>43841</v>
       </c>
       <c r="C193" s="12">
@@ -7311,7 +7313,7 @@
       <c r="A194" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B194" s="20">
+      <c r="B194" s="19">
         <v>43842</v>
       </c>
       <c r="C194" s="12">
@@ -7346,7 +7348,7 @@
       <c r="A195" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B195" s="20">
+      <c r="B195" s="19">
         <v>43843</v>
       </c>
       <c r="C195" s="12">
@@ -7381,7 +7383,7 @@
       <c r="A196" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B196" s="20">
+      <c r="B196" s="19">
         <v>43844</v>
       </c>
       <c r="C196" s="12">
@@ -7416,7 +7418,7 @@
       <c r="A197" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B197" s="20">
+      <c r="B197" s="19">
         <v>43845</v>
       </c>
       <c r="C197" s="12">
@@ -7451,7 +7453,7 @@
       <c r="A198" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B198" s="20">
+      <c r="B198" s="19">
         <v>43846</v>
       </c>
       <c r="C198" s="12">
@@ -7486,7 +7488,7 @@
       <c r="A199" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B199" s="20">
+      <c r="B199" s="19">
         <v>43847</v>
       </c>
       <c r="C199" s="12">
@@ -7521,7 +7523,7 @@
       <c r="A200" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B200" s="20">
+      <c r="B200" s="19">
         <v>43848</v>
       </c>
       <c r="C200" s="12">
@@ -7556,7 +7558,7 @@
       <c r="A201" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B201" s="20">
+      <c r="B201" s="19">
         <v>43849</v>
       </c>
       <c r="C201" s="12">
@@ -7591,7 +7593,7 @@
       <c r="A202" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B202" s="20">
+      <c r="B202" s="19">
         <v>43850</v>
       </c>
       <c r="C202" s="12">
@@ -7626,7 +7628,7 @@
       <c r="A203" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B203" s="20">
+      <c r="B203" s="19">
         <v>43851</v>
       </c>
       <c r="C203" s="12">
@@ -7661,7 +7663,7 @@
       <c r="A204" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B204" s="20">
+      <c r="B204" s="19">
         <v>43852</v>
       </c>
       <c r="C204" s="12">
@@ -7696,7 +7698,7 @@
       <c r="A205" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B205" s="20">
+      <c r="B205" s="19">
         <v>43853</v>
       </c>
       <c r="C205" s="12">
@@ -7731,7 +7733,7 @@
       <c r="A206" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B206" s="20">
+      <c r="B206" s="19">
         <v>43854</v>
       </c>
       <c r="C206" s="12">
@@ -7766,7 +7768,7 @@
       <c r="A207" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B207" s="20">
+      <c r="B207" s="19">
         <v>43855</v>
       </c>
       <c r="C207" s="12">
@@ -7801,7 +7803,7 @@
       <c r="A208" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B208" s="20">
+      <c r="B208" s="19">
         <v>43856</v>
       </c>
       <c r="C208" s="12">
@@ -7836,7 +7838,7 @@
       <c r="A209" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B209" s="20">
+      <c r="B209" s="19">
         <v>43857</v>
       </c>
       <c r="C209" s="12">
@@ -7871,7 +7873,7 @@
       <c r="A210" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B210" s="20">
+      <c r="B210" s="19">
         <v>43858</v>
       </c>
       <c r="C210" s="12">
@@ -7906,7 +7908,7 @@
       <c r="A211" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B211" s="20">
+      <c r="B211" s="19">
         <v>43859</v>
       </c>
       <c r="C211" s="12">
@@ -7941,7 +7943,7 @@
       <c r="A212" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B212" s="20">
+      <c r="B212" s="19">
         <v>43860</v>
       </c>
       <c r="C212" s="12">
@@ -7976,7 +7978,7 @@
       <c r="A213" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B213" s="20">
+      <c r="B213" s="19">
         <v>43861</v>
       </c>
       <c r="C213" s="12">
@@ -8011,7 +8013,7 @@
       <c r="A214" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B214" s="20">
+      <c r="B214" s="19">
         <v>43862</v>
       </c>
       <c r="C214" s="12">
@@ -8046,7 +8048,7 @@
       <c r="A215" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B215" s="20">
+      <c r="B215" s="19">
         <v>43863</v>
       </c>
       <c r="C215" s="12">
@@ -8081,7 +8083,7 @@
       <c r="A216" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B216" s="20">
+      <c r="B216" s="19">
         <v>43864</v>
       </c>
       <c r="C216" s="12">
@@ -8116,7 +8118,7 @@
       <c r="A217" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B217" s="20">
+      <c r="B217" s="19">
         <v>43865</v>
       </c>
       <c r="C217" s="12">
@@ -8151,7 +8153,7 @@
       <c r="A218" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B218" s="20">
+      <c r="B218" s="19">
         <v>43866</v>
       </c>
       <c r="C218" s="12">
@@ -8186,7 +8188,7 @@
       <c r="A219" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B219" s="20">
+      <c r="B219" s="19">
         <v>43867</v>
       </c>
       <c r="C219" s="12">
@@ -8221,7 +8223,7 @@
       <c r="A220" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B220" s="20">
+      <c r="B220" s="19">
         <v>43868</v>
       </c>
       <c r="C220" s="12">
@@ -8256,7 +8258,7 @@
       <c r="A221" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B221" s="20">
+      <c r="B221" s="19">
         <v>43869</v>
       </c>
       <c r="C221" s="12">
@@ -9764,7 +9766,7 @@
       <c r="B264" s="8">
         <v>43912</v>
       </c>
-      <c r="C264" s="21">
+      <c r="C264" s="20">
         <v>0.30696204964384161</v>
       </c>
       <c r="D264" s="1"/>
@@ -9799,7 +9801,7 @@
       <c r="B265" s="8">
         <v>43913</v>
       </c>
-      <c r="C265" s="21">
+      <c r="C265" s="20">
         <v>0.40122092003475646</v>
       </c>
       <c r="D265" s="1"/>
@@ -9834,7 +9836,7 @@
       <c r="B266" s="8">
         <v>43914</v>
       </c>
-      <c r="C266" s="21">
+      <c r="C266" s="20">
         <v>0.79824670912151552</v>
       </c>
       <c r="D266" s="1"/>
@@ -9869,7 +9871,7 @@
       <c r="B267" s="8">
         <v>43915</v>
       </c>
-      <c r="C267" s="21">
+      <c r="C267" s="20">
         <v>0.53261498243103889</v>
       </c>
       <c r="D267" s="1"/>
@@ -9904,7 +9906,7 @@
       <c r="B268" s="8">
         <v>43916</v>
       </c>
-      <c r="C268" s="21">
+      <c r="C268" s="20">
         <v>0.62138312919059635</v>
       </c>
       <c r="D268" s="1"/>
@@ -9939,7 +9941,7 @@
       <c r="B269" s="8">
         <v>43917</v>
       </c>
-      <c r="C269" s="21">
+      <c r="C269" s="20">
         <v>0.77834847176806521</v>
       </c>
       <c r="D269" s="1"/>
@@ -9974,7 +9976,7 @@
       <c r="B270" s="8">
         <v>43918</v>
       </c>
-      <c r="C270" s="21">
+      <c r="C270" s="20">
         <v>0.40278433646178341</v>
       </c>
       <c r="D270" s="1"/>
@@ -10009,7 +10011,7 @@
       <c r="B271" s="8">
         <v>43919</v>
       </c>
-      <c r="C271" s="21">
+      <c r="C271" s="20">
         <v>0.23382529426760165</v>
       </c>
       <c r="D271" s="1"/>
@@ -10044,7 +10046,7 @@
       <c r="B272" s="8">
         <v>43920</v>
       </c>
-      <c r="C272" s="21">
+      <c r="C272" s="20">
         <v>0.17698394856866556</v>
       </c>
       <c r="D272" s="1"/>
@@ -10079,7 +10081,7 @@
       <c r="B273" s="8">
         <v>43921</v>
       </c>
-      <c r="C273" s="21">
+      <c r="C273" s="20">
         <v>0.26022600214366559</v>
       </c>
       <c r="D273" s="1"/>
@@ -10114,7 +10116,7 @@
       <c r="B274" s="8">
         <v>43922</v>
       </c>
-      <c r="C274" s="21">
+      <c r="C274" s="20">
         <v>0.29904432187031033</v>
       </c>
       <c r="D274" s="1"/>
@@ -10149,7 +10151,7 @@
       <c r="B275" s="8">
         <v>43923</v>
       </c>
-      <c r="C275" s="21">
+      <c r="C275" s="20">
         <v>0.38052359030468075</v>
       </c>
       <c r="D275" s="6"/>
@@ -11759,7 +11761,7 @@
       <c r="B321" s="8">
         <v>43969</v>
       </c>
-      <c r="C321" s="19">
+      <c r="C321" s="18">
         <v>0.37083291268006313</v>
       </c>
       <c r="D321" s="1"/>
@@ -11794,7 +11796,7 @@
       <c r="B322" s="8">
         <v>43970</v>
       </c>
-      <c r="C322" s="19">
+      <c r="C322" s="18">
         <v>0.1554394139606054</v>
       </c>
       <c r="D322" s="1"/>
@@ -11829,7 +11831,7 @@
       <c r="B323" s="8">
         <v>43971</v>
       </c>
-      <c r="C323" s="19">
+      <c r="C323" s="18">
         <v>0.50819085152919652</v>
       </c>
       <c r="D323" s="1"/>
@@ -11864,7 +11866,7 @@
       <c r="B324" s="8">
         <v>43972</v>
       </c>
-      <c r="C324" s="19">
+      <c r="C324" s="18">
         <v>0.97926335816194932</v>
       </c>
       <c r="D324" s="1"/>
@@ -11899,7 +11901,7 @@
       <c r="B325" s="8">
         <v>43973</v>
       </c>
-      <c r="C325" s="19">
+      <c r="C325" s="18">
         <v>0.96707970332129289</v>
       </c>
       <c r="D325" s="1"/>
@@ -11934,7 +11936,7 @@
       <c r="B326" s="8">
         <v>43974</v>
       </c>
-      <c r="C326" s="19">
+      <c r="C326" s="18">
         <v>0.85579504577009513</v>
       </c>
       <c r="D326" s="1"/>
@@ -11969,7 +11971,7 @@
       <c r="B327" s="8">
         <v>43975</v>
       </c>
-      <c r="C327" s="19">
+      <c r="C327" s="18">
         <v>0.15999669642445113</v>
       </c>
       <c r="D327" s="6"/>
@@ -12004,7 +12006,7 @@
       <c r="B328" s="8">
         <v>43976</v>
       </c>
-      <c r="C328" s="19">
+      <c r="C328" s="18">
         <v>0.11764904838159539</v>
       </c>
       <c r="D328" s="1"/>
@@ -12039,7 +12041,7 @@
       <c r="B329" s="8">
         <v>43977</v>
       </c>
-      <c r="C329" s="19">
+      <c r="C329" s="18">
         <v>0.22767180825726052</v>
       </c>
       <c r="D329" s="1"/>
@@ -12074,7 +12076,7 @@
       <c r="B330" s="8">
         <v>43978</v>
       </c>
-      <c r="C330" s="19">
+      <c r="C330" s="18">
         <v>0.20702937438922503</v>
       </c>
       <c r="D330" s="1"/>
@@ -12109,7 +12111,7 @@
       <c r="B331" s="8">
         <v>43979</v>
       </c>
-      <c r="C331" s="19">
+      <c r="C331" s="18">
         <v>0.17807160403336822</v>
       </c>
       <c r="D331" s="1"/>
@@ -12144,7 +12146,7 @@
       <c r="B332" s="8">
         <v>43980</v>
       </c>
-      <c r="C332" s="19">
+      <c r="C332" s="18">
         <v>0.18132065839838882</v>
       </c>
       <c r="D332" s="1"/>
@@ -12179,7 +12181,7 @@
       <c r="B333" s="8">
         <v>43981</v>
       </c>
-      <c r="C333" s="19">
+      <c r="C333" s="18">
         <v>0.15043863303740543</v>
       </c>
       <c r="D333" s="1"/>
@@ -12214,7 +12216,7 @@
       <c r="B334" s="8">
         <v>43982</v>
       </c>
-      <c r="C334" s="19">
+      <c r="C334" s="18">
         <v>0.12801626394462842</v>
       </c>
       <c r="D334" s="6"/>
@@ -12249,7 +12251,7 @@
       <c r="B335" s="8">
         <v>43983</v>
       </c>
-      <c r="C335" s="19">
+      <c r="C335" s="18">
         <v>0.13800627741411528</v>
       </c>
       <c r="D335" s="1"/>
@@ -12284,7 +12286,7 @@
       <c r="B336" s="8">
         <v>43984</v>
       </c>
-      <c r="C336" s="19">
+      <c r="C336" s="18">
         <v>0.13231283945782799</v>
       </c>
       <c r="D336" s="1"/>
@@ -12319,7 +12321,7 @@
       <c r="B337" s="8">
         <v>43985</v>
       </c>
-      <c r="C337" s="19">
+      <c r="C337" s="18">
         <v>0.1194082558533115</v>
       </c>
       <c r="D337" s="1"/>
@@ -12354,7 +12356,7 @@
       <c r="B338" s="8">
         <v>43986</v>
       </c>
-      <c r="C338" s="19">
+      <c r="C338" s="18">
         <v>0.16149628784517653</v>
       </c>
       <c r="D338" s="1"/>
@@ -12389,7 +12391,7 @@
       <c r="B339" s="8">
         <v>43987</v>
       </c>
-      <c r="C339" s="19">
+      <c r="C339" s="18">
         <v>0.16349690155290705</v>
       </c>
       <c r="D339" s="1"/>
@@ -12424,7 +12426,7 @@
       <c r="B340" s="8">
         <v>43988</v>
       </c>
-      <c r="C340" s="19">
+      <c r="C340" s="18">
         <v>0.22430112737379229</v>
       </c>
       <c r="D340" s="6"/>
@@ -12459,7 +12461,7 @@
       <c r="B341" s="8">
         <v>43989</v>
       </c>
-      <c r="C341" s="19">
+      <c r="C341" s="18">
         <v>0.22838171258307866</v>
       </c>
       <c r="D341" s="1"/>
@@ -12483,7 +12485,7 @@
       <c r="V341" s="2"/>
       <c r="W341" s="2"/>
       <c r="X341" s="2"/>
-      <c r="Y341" s="19"/>
+      <c r="Y341" s="18"/>
       <c r="Z341" s="2"/>
       <c r="AA341" s="2"/>
       <c r="AB341" s="7"/>
@@ -12496,7 +12498,7 @@
       <c r="B342" s="8">
         <v>43990</v>
       </c>
-      <c r="C342" s="19">
+      <c r="C342" s="18">
         <v>0.21485270202767642</v>
       </c>
       <c r="D342" s="1"/>
@@ -12520,7 +12522,7 @@
       <c r="V342" s="2"/>
       <c r="W342" s="2"/>
       <c r="X342" s="2"/>
-      <c r="Y342" s="19"/>
+      <c r="Y342" s="18"/>
       <c r="Z342" s="2"/>
       <c r="AA342" s="2"/>
       <c r="AB342" s="7"/>
@@ -12533,7 +12535,7 @@
       <c r="B343" s="8">
         <v>43991</v>
       </c>
-      <c r="C343" s="19">
+      <c r="C343" s="18">
         <v>0.32536585980822613</v>
       </c>
       <c r="D343" s="1"/>
@@ -12552,12 +12554,12 @@
       <c r="Q343" s="2"/>
       <c r="R343" s="2"/>
       <c r="S343" s="2"/>
-      <c r="T343" s="19"/>
+      <c r="T343" s="18"/>
       <c r="U343" s="2"/>
       <c r="V343" s="2"/>
       <c r="W343" s="2"/>
       <c r="X343" s="2"/>
-      <c r="Y343" s="19"/>
+      <c r="Y343" s="18"/>
       <c r="Z343" s="2"/>
       <c r="AA343" s="2"/>
       <c r="AB343" s="7"/>
@@ -12570,7 +12572,7 @@
       <c r="B344" s="8">
         <v>43992</v>
       </c>
-      <c r="C344" s="19">
+      <c r="C344" s="18">
         <v>0.23773168777702364</v>
       </c>
       <c r="D344" s="1"/>
@@ -12589,12 +12591,12 @@
       <c r="Q344" s="2"/>
       <c r="R344" s="2"/>
       <c r="S344" s="2"/>
-      <c r="T344" s="19"/>
+      <c r="T344" s="18"/>
       <c r="U344" s="2"/>
       <c r="V344" s="2"/>
       <c r="W344" s="2"/>
       <c r="X344" s="2"/>
-      <c r="Y344" s="19"/>
+      <c r="Y344" s="18"/>
       <c r="Z344" s="2"/>
       <c r="AA344" s="2"/>
       <c r="AB344" s="7"/>
@@ -12607,7 +12609,7 @@
       <c r="B345" s="8">
         <v>43993</v>
       </c>
-      <c r="C345" s="19">
+      <c r="C345" s="18">
         <v>0.35381781003775015</v>
       </c>
       <c r="D345" s="1"/>
@@ -12631,7 +12633,7 @@
       <c r="V345" s="2"/>
       <c r="W345" s="2"/>
       <c r="X345" s="2"/>
-      <c r="Y345" s="19"/>
+      <c r="Y345" s="18"/>
       <c r="Z345" s="2"/>
       <c r="AA345" s="2"/>
       <c r="AB345" s="7"/>
@@ -12644,7 +12646,7 @@
       <c r="B346" s="8">
         <v>43994</v>
       </c>
-      <c r="C346" s="19">
+      <c r="C346" s="18">
         <v>0.20251615557568392</v>
       </c>
       <c r="D346" s="6"/>
@@ -12663,12 +12665,12 @@
       <c r="Q346" s="2"/>
       <c r="R346" s="2"/>
       <c r="S346" s="2"/>
-      <c r="T346" s="19"/>
+      <c r="T346" s="18"/>
       <c r="U346" s="2"/>
       <c r="V346" s="2"/>
       <c r="W346" s="2"/>
       <c r="X346" s="2"/>
-      <c r="Y346" s="19"/>
+      <c r="Y346" s="18"/>
       <c r="Z346" s="2"/>
       <c r="AA346" s="2"/>
       <c r="AB346" s="7"/>
@@ -12681,7 +12683,7 @@
       <c r="B347" s="8">
         <v>43995</v>
       </c>
-      <c r="C347" s="19">
+      <c r="C347" s="18">
         <v>0.18189728571354846</v>
       </c>
       <c r="D347" s="1"/>
@@ -12705,7 +12707,7 @@
       <c r="V347" s="2"/>
       <c r="W347" s="2"/>
       <c r="X347" s="2"/>
-      <c r="Y347" s="19"/>
+      <c r="Y347" s="18"/>
       <c r="Z347" s="2"/>
       <c r="AA347" s="2"/>
       <c r="AB347" s="7"/>
@@ -12718,7 +12720,7 @@
       <c r="B348" s="8">
         <v>43996</v>
       </c>
-      <c r="C348" s="19">
+      <c r="C348" s="18">
         <v>0.12630748908405504</v>
       </c>
       <c r="D348" s="1"/>
@@ -12742,7 +12744,7 @@
       <c r="V348" s="2"/>
       <c r="W348" s="2"/>
       <c r="X348" s="2"/>
-      <c r="Y348" s="19"/>
+      <c r="Y348" s="18"/>
       <c r="Z348" s="2"/>
       <c r="AA348" s="2"/>
       <c r="AB348" s="7"/>
@@ -12755,7 +12757,7 @@
       <c r="B349" s="8">
         <v>43997</v>
       </c>
-      <c r="C349" s="19">
+      <c r="C349" s="18">
         <v>0.15664383967645612</v>
       </c>
       <c r="D349" s="1"/>
@@ -12774,12 +12776,12 @@
       <c r="Q349" s="2"/>
       <c r="R349" s="2"/>
       <c r="S349" s="2"/>
-      <c r="T349" s="19"/>
+      <c r="T349" s="18"/>
       <c r="U349" s="2"/>
       <c r="V349" s="2"/>
       <c r="W349" s="2"/>
       <c r="X349" s="2"/>
-      <c r="Y349" s="19"/>
+      <c r="Y349" s="18"/>
       <c r="Z349" s="2"/>
       <c r="AA349" s="2"/>
       <c r="AB349" s="7"/>
@@ -12792,7 +12794,7 @@
       <c r="B350" s="8">
         <v>43998</v>
       </c>
-      <c r="C350" s="19">
+      <c r="C350" s="18">
         <v>0.27419109401868741</v>
       </c>
       <c r="D350" s="1"/>
@@ -12811,12 +12813,12 @@
       <c r="Q350" s="2"/>
       <c r="R350" s="2"/>
       <c r="S350" s="2"/>
-      <c r="T350" s="19"/>
+      <c r="T350" s="18"/>
       <c r="U350" s="2"/>
       <c r="V350" s="2"/>
       <c r="W350" s="2"/>
       <c r="X350" s="2"/>
-      <c r="Y350" s="19"/>
+      <c r="Y350" s="18"/>
       <c r="Z350" s="2"/>
       <c r="AA350" s="2"/>
       <c r="AB350" s="7"/>
@@ -12829,7 +12831,7 @@
       <c r="B351" s="8">
         <v>43999</v>
       </c>
-      <c r="C351" s="19">
+      <c r="C351" s="18">
         <v>0.1332312275851073</v>
       </c>
       <c r="D351" s="1"/>
@@ -12848,12 +12850,12 @@
       <c r="Q351" s="2"/>
       <c r="R351" s="2"/>
       <c r="S351" s="2"/>
-      <c r="T351" s="19"/>
+      <c r="T351" s="18"/>
       <c r="U351" s="2"/>
       <c r="V351" s="2"/>
       <c r="W351" s="2"/>
       <c r="X351" s="2"/>
-      <c r="Y351" s="19"/>
+      <c r="Y351" s="18"/>
       <c r="Z351" s="2"/>
       <c r="AA351" s="2"/>
       <c r="AB351" s="7"/>
@@ -12866,7 +12868,7 @@
       <c r="B352" s="8">
         <v>44000</v>
       </c>
-      <c r="C352" s="19">
+      <c r="C352" s="18">
         <v>0.16169845734594498</v>
       </c>
       <c r="D352" s="6"/>
@@ -12885,12 +12887,12 @@
       <c r="Q352" s="2"/>
       <c r="R352" s="2"/>
       <c r="S352" s="2"/>
-      <c r="T352" s="19"/>
+      <c r="T352" s="18"/>
       <c r="U352" s="2"/>
       <c r="V352" s="2"/>
       <c r="W352" s="2"/>
       <c r="X352" s="2"/>
-      <c r="Y352" s="19"/>
+      <c r="Y352" s="18"/>
       <c r="Z352" s="2"/>
       <c r="AA352" s="2"/>
       <c r="AB352" s="7"/>
@@ -12903,7 +12905,7 @@
       <c r="B353" s="8">
         <v>44001</v>
       </c>
-      <c r="C353" s="19">
+      <c r="C353" s="18">
         <v>0.14432273798106138</v>
       </c>
       <c r="D353" s="1"/>
@@ -12927,7 +12929,7 @@
       <c r="V353" s="2"/>
       <c r="W353" s="2"/>
       <c r="X353" s="2"/>
-      <c r="Y353" s="19"/>
+      <c r="Y353" s="18"/>
       <c r="Z353" s="2"/>
       <c r="AA353" s="2"/>
       <c r="AB353" s="7"/>
@@ -12940,7 +12942,7 @@
       <c r="B354" s="8">
         <v>44002</v>
       </c>
-      <c r="C354" s="19">
+      <c r="C354" s="18">
         <v>0.20711780804999677</v>
       </c>
       <c r="D354" s="1"/>
@@ -12964,7 +12966,7 @@
       <c r="V354" s="2"/>
       <c r="W354" s="2"/>
       <c r="X354" s="2"/>
-      <c r="Y354" s="19"/>
+      <c r="Y354" s="18"/>
       <c r="Z354" s="2"/>
       <c r="AA354" s="2"/>
       <c r="AB354" s="7"/>
@@ -12977,7 +12979,7 @@
       <c r="B355" s="8">
         <v>44003</v>
       </c>
-      <c r="C355" s="19">
+      <c r="C355" s="18">
         <v>0.1545301924301907</v>
       </c>
       <c r="D355" s="1"/>
@@ -12996,12 +12998,12 @@
       <c r="Q355" s="2"/>
       <c r="R355" s="2"/>
       <c r="S355" s="2"/>
-      <c r="T355" s="19"/>
+      <c r="T355" s="18"/>
       <c r="U355" s="2"/>
       <c r="V355" s="2"/>
       <c r="W355" s="2"/>
       <c r="X355" s="2"/>
-      <c r="Y355" s="19"/>
+      <c r="Y355" s="18"/>
       <c r="Z355" s="2"/>
       <c r="AA355" s="2"/>
       <c r="AB355" s="7"/>
@@ -13014,7 +13016,7 @@
       <c r="B356" s="8">
         <v>44004</v>
       </c>
-      <c r="C356" s="19">
+      <c r="C356" s="18">
         <v>0.15957057412195624</v>
       </c>
       <c r="D356" s="1"/>
@@ -13033,12 +13035,12 @@
       <c r="Q356" s="2"/>
       <c r="R356" s="2"/>
       <c r="S356" s="2"/>
-      <c r="T356" s="19"/>
+      <c r="T356" s="18"/>
       <c r="U356" s="2"/>
       <c r="V356" s="2"/>
       <c r="W356" s="2"/>
       <c r="X356" s="2"/>
-      <c r="Y356" s="19"/>
+      <c r="Y356" s="18"/>
       <c r="Z356" s="2"/>
       <c r="AA356" s="2"/>
       <c r="AB356" s="7"/>
@@ -13051,7 +13053,7 @@
       <c r="B357" s="8">
         <v>44005</v>
       </c>
-      <c r="C357" s="19">
+      <c r="C357" s="18">
         <v>0.15917492961194732</v>
       </c>
       <c r="D357" s="1"/>
@@ -13070,12 +13072,12 @@
       <c r="Q357" s="2"/>
       <c r="R357" s="2"/>
       <c r="S357" s="2"/>
-      <c r="T357" s="19"/>
+      <c r="T357" s="18"/>
       <c r="U357" s="2"/>
       <c r="V357" s="2"/>
       <c r="W357" s="2"/>
       <c r="X357" s="2"/>
-      <c r="Y357" s="19"/>
+      <c r="Y357" s="18"/>
       <c r="Z357" s="2"/>
       <c r="AA357" s="2"/>
       <c r="AB357" s="7"/>
@@ -13088,7 +13090,7 @@
       <c r="B358" s="8">
         <v>44006</v>
       </c>
-      <c r="C358" s="19">
+      <c r="C358" s="18">
         <v>0.19053888194921231</v>
       </c>
       <c r="D358" s="6"/>
@@ -13107,12 +13109,12 @@
       <c r="Q358" s="2"/>
       <c r="R358" s="2"/>
       <c r="S358" s="2"/>
-      <c r="T358" s="19"/>
+      <c r="T358" s="18"/>
       <c r="U358" s="2"/>
       <c r="V358" s="2"/>
       <c r="W358" s="2"/>
       <c r="X358" s="2"/>
-      <c r="Y358" s="19"/>
+      <c r="Y358" s="18"/>
       <c r="Z358" s="2"/>
       <c r="AA358" s="2"/>
       <c r="AB358" s="7"/>
@@ -13125,7 +13127,7 @@
       <c r="B359" s="8">
         <v>44007</v>
       </c>
-      <c r="C359" s="19">
+      <c r="C359" s="18">
         <v>0.1709967775265942</v>
       </c>
       <c r="D359" s="1"/>
@@ -13149,7 +13151,7 @@
       <c r="V359" s="2"/>
       <c r="W359" s="2"/>
       <c r="X359" s="2"/>
-      <c r="Y359" s="19"/>
+      <c r="Y359" s="18"/>
       <c r="Z359" s="2"/>
       <c r="AA359" s="2"/>
       <c r="AB359" s="7"/>
@@ -13162,7 +13164,7 @@
       <c r="B360" s="8">
         <v>44008</v>
       </c>
-      <c r="C360" s="19">
+      <c r="C360" s="18">
         <v>0.15193171470159281</v>
       </c>
       <c r="D360" s="1"/>
@@ -13186,7 +13188,7 @@
       <c r="V360" s="2"/>
       <c r="W360" s="2"/>
       <c r="X360" s="2"/>
-      <c r="Y360" s="19"/>
+      <c r="Y360" s="18"/>
       <c r="Z360" s="2"/>
       <c r="AA360" s="2"/>
       <c r="AB360" s="7"/>
@@ -13199,7 +13201,7 @@
       <c r="B361" s="8">
         <v>44009</v>
       </c>
-      <c r="C361" s="19">
+      <c r="C361" s="18">
         <v>0.1865661198641772</v>
       </c>
       <c r="D361" s="1"/>
@@ -13218,12 +13220,12 @@
       <c r="Q361" s="2"/>
       <c r="R361" s="2"/>
       <c r="S361" s="2"/>
-      <c r="T361" s="19"/>
+      <c r="T361" s="18"/>
       <c r="U361" s="2"/>
       <c r="V361" s="2"/>
       <c r="W361" s="2"/>
       <c r="X361" s="2"/>
-      <c r="Y361" s="19"/>
+      <c r="Y361" s="18"/>
       <c r="Z361" s="2"/>
       <c r="AA361" s="2"/>
       <c r="AB361" s="7"/>
@@ -13236,7 +13238,7 @@
       <c r="B362" s="8">
         <v>44010</v>
       </c>
-      <c r="C362" s="19">
+      <c r="C362" s="18">
         <v>0.14406344167150847</v>
       </c>
       <c r="D362" s="1"/>
@@ -13255,12 +13257,12 @@
       <c r="Q362" s="2"/>
       <c r="R362" s="2"/>
       <c r="S362" s="2"/>
-      <c r="T362" s="19"/>
+      <c r="T362" s="18"/>
       <c r="U362" s="2"/>
       <c r="V362" s="2"/>
       <c r="W362" s="2"/>
       <c r="X362" s="2"/>
-      <c r="Y362" s="19"/>
+      <c r="Y362" s="18"/>
       <c r="Z362" s="2"/>
       <c r="AA362" s="2"/>
       <c r="AB362" s="7"/>
@@ -13273,7 +13275,7 @@
       <c r="B363" s="8">
         <v>44011</v>
       </c>
-      <c r="C363" s="19">
+      <c r="C363" s="18">
         <v>0.294939130550043</v>
       </c>
       <c r="D363" s="1"/>
@@ -13292,21 +13294,27 @@
       <c r="Q363" s="2"/>
       <c r="R363" s="2"/>
       <c r="S363" s="2"/>
-      <c r="T363" s="19"/>
+      <c r="T363" s="18"/>
       <c r="U363" s="2"/>
       <c r="V363" s="2"/>
       <c r="W363" s="2"/>
       <c r="X363" s="2"/>
-      <c r="Y363" s="19"/>
+      <c r="Y363" s="18"/>
       <c r="Z363" s="2"/>
       <c r="AA363" s="2"/>
       <c r="AB363" s="7"/>
       <c r="AC363" s="7"/>
     </row>
     <row r="364" spans="1:29" x14ac:dyDescent="0.5">
-      <c r="A364" s="17"/>
-      <c r="B364" s="1"/>
-      <c r="C364" s="18"/>
+      <c r="A364" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B364" s="8">
+        <v>43831</v>
+      </c>
+      <c r="C364" s="18">
+        <v>0.2496051993211684</v>
+      </c>
       <c r="D364" s="6"/>
       <c r="E364" s="1"/>
       <c r="F364" s="2"/>
@@ -13323,17 +13331,1997 @@
       <c r="Q364" s="2"/>
       <c r="R364" s="2"/>
       <c r="S364" s="2"/>
-      <c r="T364" s="19"/>
+      <c r="T364" s="18"/>
       <c r="U364" s="2"/>
       <c r="V364" s="2"/>
       <c r="W364" s="2"/>
       <c r="X364" s="2"/>
-      <c r="Y364" s="19"/>
+      <c r="Y364" s="18"/>
       <c r="Z364" s="2"/>
       <c r="AA364" s="2"/>
       <c r="AB364" s="7"/>
       <c r="AC364" s="7"/>
     </row>
+    <row r="365" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A365" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B365" s="6">
+        <v>43832</v>
+      </c>
+      <c r="C365" s="7">
+        <v>0.245345348684398</v>
+      </c>
+    </row>
+    <row r="366" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A366" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B366" s="6">
+        <v>43833</v>
+      </c>
+      <c r="C366" s="7">
+        <v>0.34954632546645392</v>
+      </c>
+    </row>
+    <row r="367" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A367" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B367" s="6">
+        <v>43834</v>
+      </c>
+      <c r="C367" s="7">
+        <v>0.43505086713689728</v>
+      </c>
+    </row>
+    <row r="368" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A368" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B368" s="6">
+        <v>43835</v>
+      </c>
+      <c r="C368" s="7">
+        <v>0.60216258047060822</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A369" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B369" s="6">
+        <v>43836</v>
+      </c>
+      <c r="C369" s="7">
+        <v>0.99260094847756264</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A370" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B370" s="6">
+        <v>43837</v>
+      </c>
+      <c r="C370" s="7">
+        <v>0.67263590304063992</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A371" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B371" s="6">
+        <v>43838</v>
+      </c>
+      <c r="C371" s="7">
+        <v>0.52865558266372403</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A372" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B372" s="6">
+        <v>43839</v>
+      </c>
+      <c r="C372" s="7">
+        <v>0.28403388708156774</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A373" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B373" s="6">
+        <v>43840</v>
+      </c>
+      <c r="C373" s="7">
+        <v>0.3151102664726132</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A374" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B374" s="6">
+        <v>43841</v>
+      </c>
+      <c r="C374" s="7">
+        <v>0.74597441902919981</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A375" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B375" s="6">
+        <v>43842</v>
+      </c>
+      <c r="C375" s="7">
+        <v>0.65177262238670086</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A376" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B376" s="6">
+        <v>43843</v>
+      </c>
+      <c r="C376" s="7">
+        <v>0.55625623711246375</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A377" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B377" s="6">
+        <v>43844</v>
+      </c>
+      <c r="C377" s="7">
+        <v>0.3287985488689712</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A378" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B378" s="6">
+        <v>43845</v>
+      </c>
+      <c r="C378" s="7">
+        <v>0.25292770751167781</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A379" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B379" s="6">
+        <v>43846</v>
+      </c>
+      <c r="C379" s="7">
+        <v>0.29672080075050761</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A380" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B380" s="6">
+        <v>43847</v>
+      </c>
+      <c r="C380" s="7">
+        <v>0.13510288085107278</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A381" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B381" s="6">
+        <v>43848</v>
+      </c>
+      <c r="C381" s="7">
+        <v>0.2879812125095812</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A382" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B382" s="6">
+        <v>43849</v>
+      </c>
+      <c r="C382" s="7">
+        <v>0.46876927798532453</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A383" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B383" s="6">
+        <v>43850</v>
+      </c>
+      <c r="C383" s="7">
+        <v>0.12368323546620789</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A384" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B384" s="6">
+        <v>43851</v>
+      </c>
+      <c r="C384" s="7">
+        <v>0.37795170860935923</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A385" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B385" s="6">
+        <v>43852</v>
+      </c>
+      <c r="C385" s="7">
+        <v>0.21764816703561143</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A386" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B386" s="6">
+        <v>43853</v>
+      </c>
+      <c r="C386" s="7">
+        <v>0.14400473462773314</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A387" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B387" s="6">
+        <v>43854</v>
+      </c>
+      <c r="C387" s="7">
+        <v>0.47814610692339093</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A388" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B388" s="6">
+        <v>43855</v>
+      </c>
+      <c r="C388" s="7">
+        <v>0.15943347803558494</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A389" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B389" s="6">
+        <v>43856</v>
+      </c>
+      <c r="C389" s="7">
+        <v>0.13025233417401619</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A390" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B390" s="6">
+        <v>43857</v>
+      </c>
+      <c r="C390" s="7">
+        <v>0.14849182142358811</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A391" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B391" s="6">
+        <v>43858</v>
+      </c>
+      <c r="C391" s="7">
+        <v>0.29909446572399018</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A392" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B392" s="6">
+        <v>43859</v>
+      </c>
+      <c r="C392" s="7">
+        <v>0.97780146003716861</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A393" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B393" s="6">
+        <v>43860</v>
+      </c>
+      <c r="C393" s="7">
+        <v>0.64205883347883697</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A394" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B394" s="6">
+        <v>43861</v>
+      </c>
+      <c r="C394" s="7">
+        <v>0.47010629722021857</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A395" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B395" s="6">
+        <v>43862</v>
+      </c>
+      <c r="C395" s="7">
+        <v>0.83737638610158205</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A396" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B396" s="6">
+        <v>43863</v>
+      </c>
+      <c r="C396" s="7">
+        <v>0.98366122108149867</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A397" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B397" s="6">
+        <v>43864</v>
+      </c>
+      <c r="C397" s="7">
+        <v>0.59195837949166408</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A398" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B398" s="6">
+        <v>43865</v>
+      </c>
+      <c r="C398" s="7">
+        <v>0.86911731006633031</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A399" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B399" s="6">
+        <v>43866</v>
+      </c>
+      <c r="C399" s="7">
+        <v>0.5287581096747298</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A400" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B400" s="6">
+        <v>43867</v>
+      </c>
+      <c r="C400" s="7">
+        <v>0.15217924780315353</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A401" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B401" s="6">
+        <v>43868</v>
+      </c>
+      <c r="C401" s="7">
+        <v>0.10351700662767234</v>
+      </c>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A402" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B402" s="6">
+        <v>43869</v>
+      </c>
+      <c r="C402" s="7">
+        <v>0.1793085645021669</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A403" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B403" s="6">
+        <v>43870</v>
+      </c>
+      <c r="C403" s="7">
+        <v>0.24463714059352473</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A404" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B404" s="6">
+        <v>43871</v>
+      </c>
+      <c r="C404" s="7">
+        <v>0.30692074000760738</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A405" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B405" s="6">
+        <v>43872</v>
+      </c>
+      <c r="C405" s="7">
+        <v>0.38457408332939202</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A406" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B406" s="6">
+        <v>43873</v>
+      </c>
+      <c r="C406" s="7">
+        <v>0.13251152559355969</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A407" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B407" s="6">
+        <v>43874</v>
+      </c>
+      <c r="C407" s="7">
+        <v>0.16925280126881281</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A408" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B408" s="6">
+        <v>43875</v>
+      </c>
+      <c r="C408" s="7">
+        <v>0.17676972929671633</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A409" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B409" s="6">
+        <v>43876</v>
+      </c>
+      <c r="C409" s="7">
+        <v>0.12413333576476678</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A410" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B410" s="6">
+        <v>43877</v>
+      </c>
+      <c r="C410" s="7">
+        <v>0.19343373296011065</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A411" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B411" s="6">
+        <v>43878</v>
+      </c>
+      <c r="C411" s="7">
+        <v>9.0845045237237215E-2</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A412" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B412" s="6">
+        <v>43879</v>
+      </c>
+      <c r="C412" s="7">
+        <v>0.16691924312083001</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A413" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B413" s="6">
+        <v>43880</v>
+      </c>
+      <c r="C413" s="7">
+        <v>0.12314104856622678</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A414" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B414" s="6">
+        <v>43881</v>
+      </c>
+      <c r="C414" s="7">
+        <v>0.1035676371434839</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A415" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B415" s="6">
+        <v>43882</v>
+      </c>
+      <c r="C415" s="7">
+        <v>0.14022127896458161</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A416" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B416" s="6">
+        <v>43883</v>
+      </c>
+      <c r="C416" s="7">
+        <v>0.11475318207679977</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A417" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B417" s="6">
+        <v>43884</v>
+      </c>
+      <c r="C417" s="7">
+        <v>0.17890405828703732</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A418" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B418" s="6">
+        <v>43885</v>
+      </c>
+      <c r="C418" s="7">
+        <v>0.16083327389727031</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A419" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B419" s="6">
+        <v>43886</v>
+      </c>
+      <c r="C419" s="7">
+        <v>0.44390063792912549</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A420" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B420" s="6">
+        <v>43887</v>
+      </c>
+      <c r="C420" s="7">
+        <v>0.19688161817322677</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A421" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B421" s="6">
+        <v>43888</v>
+      </c>
+      <c r="C421" s="7">
+        <v>0.13510083255263633</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A422" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B422" s="6">
+        <v>43889</v>
+      </c>
+      <c r="C422" s="7">
+        <v>0.11404772117127168</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A423" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B423" s="6">
+        <v>43890</v>
+      </c>
+      <c r="C423" s="7">
+        <v>0.1347923144081925</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A424" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B424" s="6">
+        <v>43891</v>
+      </c>
+      <c r="C424" s="7">
+        <v>0.69383536985823158</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A425" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B425" s="6">
+        <v>43892</v>
+      </c>
+      <c r="C425" s="7">
+        <v>0.99134449711004036</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A426" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B426" s="6">
+        <v>43893</v>
+      </c>
+      <c r="C426" s="7">
+        <v>0.98124987821828491</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A427" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B427" s="6">
+        <v>43894</v>
+      </c>
+      <c r="C427" s="7">
+        <v>0.77056579758596877</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A428" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B428" s="6">
+        <v>43895</v>
+      </c>
+      <c r="C428" s="7">
+        <v>0.35801605399112152</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A429" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B429" s="6">
+        <v>43896</v>
+      </c>
+      <c r="C429" s="7">
+        <v>9.3677796769530655E-2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A430" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B430" s="6">
+        <v>43897</v>
+      </c>
+      <c r="C430" s="7">
+        <v>8.6894284825303356E-2</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A431" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B431" s="6">
+        <v>43898</v>
+      </c>
+      <c r="C431" s="7">
+        <v>9.9836658221135605E-2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A432" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B432" s="6">
+        <v>43899</v>
+      </c>
+      <c r="C432" s="7">
+        <v>0.10083433842515703</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A433" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B433" s="6">
+        <v>43900</v>
+      </c>
+      <c r="C433" s="7">
+        <v>0.10567396300767809</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A434" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B434" s="6">
+        <v>43901</v>
+      </c>
+      <c r="C434" s="7">
+        <v>0.12102255610490484</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A435" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B435" s="6">
+        <v>43902</v>
+      </c>
+      <c r="C435" s="7">
+        <v>0.17814880144666154</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A436" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B436" s="6">
+        <v>43903</v>
+      </c>
+      <c r="C436" s="7">
+        <v>9.3135936486752974E-2</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A437" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B437" s="6">
+        <v>43904</v>
+      </c>
+      <c r="C437" s="7">
+        <v>0.10423065978238921</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A438" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B438" s="6">
+        <v>43905</v>
+      </c>
+      <c r="C438" s="7">
+        <v>0.43510315504008096</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A439" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B439" s="6">
+        <v>43906</v>
+      </c>
+      <c r="C439" s="7">
+        <v>0.13029196930813886</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A440" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B440" s="6">
+        <v>43907</v>
+      </c>
+      <c r="C440" s="7">
+        <v>0.10073757959440104</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A441" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B441" s="6">
+        <v>43908</v>
+      </c>
+      <c r="C441" s="7">
+        <v>0.10219523791606654</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A442" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B442" s="6">
+        <v>43909</v>
+      </c>
+      <c r="C442" s="7">
+        <v>9.2915276039201938E-2</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A443" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B443" s="6">
+        <v>43910</v>
+      </c>
+      <c r="C443" s="7">
+        <v>9.0471477227600974E-2</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A444" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B444" s="6">
+        <v>43911</v>
+      </c>
+      <c r="C444" s="7">
+        <v>9.2440397155101606E-2</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A445" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B445" s="6">
+        <v>43912</v>
+      </c>
+      <c r="C445" s="7">
+        <v>0.10414741047459161</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A446" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B446" s="6">
+        <v>43913</v>
+      </c>
+      <c r="C446" s="7">
+        <v>9.7979584594669281E-2</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A447" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B447" s="6">
+        <v>43914</v>
+      </c>
+      <c r="C447" s="7">
+        <v>0.13159457946928468</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A448" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B448" s="6">
+        <v>43915</v>
+      </c>
+      <c r="C448" s="7">
+        <v>0.15414825902995594</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A449" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B449" s="6">
+        <v>43916</v>
+      </c>
+      <c r="C449" s="7">
+        <v>0.17106655036745594</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A450" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B450" s="6">
+        <v>43917</v>
+      </c>
+      <c r="C450" s="7">
+        <v>0.14799704208890135</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A451" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B451" s="6">
+        <v>43918</v>
+      </c>
+      <c r="C451" s="7">
+        <v>0.12152715411954652</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A452" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B452" s="6">
+        <v>43919</v>
+      </c>
+      <c r="C452" s="7">
+        <v>0.15148685894995276</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A453" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B453" s="6">
+        <v>43920</v>
+      </c>
+      <c r="C453" s="7">
+        <v>0.65717931953432418</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A454" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B454" s="6">
+        <v>43921</v>
+      </c>
+      <c r="C454" s="7">
+        <v>0.88552474696050543</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A455" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B455" s="6">
+        <v>43922</v>
+      </c>
+      <c r="C455" s="7">
+        <v>0.48601953285460475</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A456" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B456" s="6">
+        <v>43923</v>
+      </c>
+      <c r="C456" s="7">
+        <v>0.28283292201262683</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A457" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B457" s="6">
+        <v>43924</v>
+      </c>
+      <c r="C457" s="7">
+        <v>0.2629281127926551</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A458" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B458" s="6">
+        <v>43925</v>
+      </c>
+      <c r="C458" s="7">
+        <v>0.13309099300106755</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A459" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B459" s="6">
+        <v>43926</v>
+      </c>
+      <c r="C459" s="7">
+        <v>9.8562553037100903E-2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A460" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B460" s="6">
+        <v>43927</v>
+      </c>
+      <c r="C460" s="7">
+        <v>0.42747564042152797</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A461" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B461" s="6">
+        <v>43928</v>
+      </c>
+      <c r="C461" s="7">
+        <v>0.46763015540135233</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A462" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B462" s="6">
+        <v>43929</v>
+      </c>
+      <c r="C462" s="7">
+        <v>0.9782336915309584</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A463" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B463" s="6">
+        <v>43930</v>
+      </c>
+      <c r="C463" s="7">
+        <v>0.98992457853022497</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A464" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B464" s="6">
+        <v>43931</v>
+      </c>
+      <c r="C464" s="7">
+        <v>0.10037052923773562</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A465" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B465" s="6">
+        <v>43932</v>
+      </c>
+      <c r="C465" s="7">
+        <v>9.140125737400015E-2</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A466" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B466" s="6">
+        <v>43933</v>
+      </c>
+      <c r="C466" s="7">
+        <v>0.108110743504936</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A467" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B467" s="6">
+        <v>43934</v>
+      </c>
+      <c r="C467" s="7">
+        <v>0.11158014017307624</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A468" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B468" s="6">
+        <v>43935</v>
+      </c>
+      <c r="C468" s="7">
+        <v>0.29304887769867594</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A469" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B469" s="6">
+        <v>43936</v>
+      </c>
+      <c r="C469" s="7">
+        <v>0.10327522687125598</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A470" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B470" s="6">
+        <v>43937</v>
+      </c>
+      <c r="C470" s="7">
+        <v>0.15865228101773535</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A471" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B471" s="6">
+        <v>43938</v>
+      </c>
+      <c r="C471" s="7">
+        <v>0.11710832628368352</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A472" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B472" s="6">
+        <v>43939</v>
+      </c>
+      <c r="C472" s="7">
+        <v>0.22001637243676533</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A473" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B473" s="6">
+        <v>43940</v>
+      </c>
+      <c r="C473" s="7">
+        <v>0.11362174391513193</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A474" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B474" s="6">
+        <v>43941</v>
+      </c>
+      <c r="C474" s="7">
+        <v>0.20275084313315733</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A475" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B475" s="6">
+        <v>43942</v>
+      </c>
+      <c r="C475" s="7">
+        <v>0.39817461050619712</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A476" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B476" s="6">
+        <v>43943</v>
+      </c>
+      <c r="C476" s="7">
+        <v>0.34573397315653093</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A477" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B477" s="6">
+        <v>43944</v>
+      </c>
+      <c r="C477" s="7">
+        <v>0.12004829462338175</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A478" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B478" s="6">
+        <v>43945</v>
+      </c>
+      <c r="C478" s="7">
+        <v>0.12847799729925458</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A479" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B479" s="6">
+        <v>43946</v>
+      </c>
+      <c r="C479" s="7">
+        <v>0.10035218552422992</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A480" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B480" s="6">
+        <v>43947</v>
+      </c>
+      <c r="C480" s="7">
+        <v>0.13891536502958368</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A481" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B481" s="6">
+        <v>43948</v>
+      </c>
+      <c r="C481" s="7">
+        <v>0.13142085194908831</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A482" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B482" s="6">
+        <v>43949</v>
+      </c>
+      <c r="C482" s="7">
+        <v>0.16761015909774998</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A483" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B483" s="6">
+        <v>43950</v>
+      </c>
+      <c r="C483" s="7">
+        <v>0.14624652744416428</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A484" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B484" s="6">
+        <v>43951</v>
+      </c>
+      <c r="C484" s="7">
+        <v>0.1040605736948452</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A485" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B485" s="6">
+        <v>43952</v>
+      </c>
+      <c r="C485" s="7">
+        <v>0.12353217505773692</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A486" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B486" s="6">
+        <v>43953</v>
+      </c>
+      <c r="C486" s="7">
+        <v>0.1614507022981633</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A487" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B487" s="6">
+        <v>43954</v>
+      </c>
+      <c r="C487" s="7">
+        <v>0.11522623885721321</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A488" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B488" s="6">
+        <v>43955</v>
+      </c>
+      <c r="C488" s="7">
+        <v>9.6740907855862715E-2</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A489" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B489" s="6">
+        <v>43956</v>
+      </c>
+      <c r="C489" s="7">
+        <v>9.4344376076084605E-2</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A490" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B490" s="6">
+        <v>43957</v>
+      </c>
+      <c r="C490" s="7">
+        <v>9.3285914768431386E-2</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A491" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B491" s="6">
+        <v>43958</v>
+      </c>
+      <c r="C491" s="7">
+        <v>9.7412225743168393E-2</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A492" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B492" s="6">
+        <v>43959</v>
+      </c>
+      <c r="C492" s="7">
+        <v>0.10573404927516496</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A493" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B493" s="6">
+        <v>43960</v>
+      </c>
+      <c r="C493" s="7">
+        <v>0.11691835078449006</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A494" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B494" s="6">
+        <v>43961</v>
+      </c>
+      <c r="C494" s="7">
+        <v>0.11472669644006381</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A495" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B495" s="6">
+        <v>43962</v>
+      </c>
+      <c r="C495" s="7">
+        <v>0.60405600692359684</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A496" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B496" s="6">
+        <v>43963</v>
+      </c>
+      <c r="C496" s="7">
+        <v>0.35761674640761654</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A497" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B497" s="6">
+        <v>43964</v>
+      </c>
+      <c r="C497" s="7">
+        <v>0.1014147439995027</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A498" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B498" s="6">
+        <v>43965</v>
+      </c>
+      <c r="C498" s="7">
+        <v>0.10427559715156662</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A499" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B499" s="6">
+        <v>43966</v>
+      </c>
+      <c r="C499" s="7">
+        <v>0.10623030790506649</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A500" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B500" s="6">
+        <v>43967</v>
+      </c>
+      <c r="C500" s="7">
+        <v>0.10331021780108686</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A501" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B501" s="6">
+        <v>43968</v>
+      </c>
+      <c r="C501" s="7">
+        <v>0.11015304542395961</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A502" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B502" s="6">
+        <v>43969</v>
+      </c>
+      <c r="C502" s="7">
+        <v>0.1675971135761089</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A503" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B503" s="6">
+        <v>43970</v>
+      </c>
+      <c r="C503" s="7">
+        <v>0.33289701778003156</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A504" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B504" s="6">
+        <v>43971</v>
+      </c>
+      <c r="C504" s="7">
+        <v>0.97414373857488035</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A505" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B505" s="6">
+        <v>43972</v>
+      </c>
+      <c r="C505" s="7">
+        <v>0.34794363787938071</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A506" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B506" s="6">
+        <v>43973</v>
+      </c>
+      <c r="C506" s="7">
+        <v>0.24437217715732265</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A507" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B507" s="6">
+        <v>43974</v>
+      </c>
+      <c r="C507" s="7">
+        <v>0.11177919920522686</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A508" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B508" s="6">
+        <v>43975</v>
+      </c>
+      <c r="C508" s="7">
+        <v>0.15954436901050412</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A509" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B509" s="6">
+        <v>43976</v>
+      </c>
+      <c r="C509" s="7">
+        <v>0.61655949188165327</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A510" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B510" s="6">
+        <v>43977</v>
+      </c>
+      <c r="C510" s="7">
+        <v>0.99237368981179419</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A511" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B511" s="6">
+        <v>43978</v>
+      </c>
+      <c r="C511" s="7">
+        <v>0.59336559338943062</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A512" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B512" s="6">
+        <v>43979</v>
+      </c>
+      <c r="C512" s="7">
+        <v>9.9103035140580137E-2</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A513" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B513" s="6">
+        <v>43980</v>
+      </c>
+      <c r="C513" s="7">
+        <v>9.5355208908711991E-2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A514" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B514" s="6">
+        <v>43981</v>
+      </c>
+      <c r="C514" s="7">
+        <v>0.55825225171989845</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A515" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B515" s="6">
+        <v>43982</v>
+      </c>
+      <c r="C515" s="7">
+        <v>0.19673029102756254</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A516" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B516" s="6">
+        <v>43983</v>
+      </c>
+      <c r="C516" s="7">
+        <v>0.11033416931746176</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A517" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B517" s="6">
+        <v>43984</v>
+      </c>
+      <c r="C517" s="7">
+        <v>0.134823996442792</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A518" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B518" s="6">
+        <v>43985</v>
+      </c>
+      <c r="C518" s="7">
+        <v>0.2434233207461857</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A519" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B519" s="6">
+        <v>43986</v>
+      </c>
+      <c r="C519" s="7">
+        <v>0.39473330388183547</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A520" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B520" s="6">
+        <v>43987</v>
+      </c>
+      <c r="C520" s="7">
+        <v>9.8780501431367643E-2</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A521" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B521" s="6">
+        <v>43988</v>
+      </c>
+      <c r="C521" s="7">
+        <v>0.10633028922796058</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A522" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B522" s="6">
+        <v>43989</v>
+      </c>
+      <c r="C522" s="7">
+        <v>0.10535739406811488</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A523" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B523" s="6">
+        <v>43990</v>
+      </c>
+      <c r="C523" s="7">
+        <v>0.30323164248393181</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A524" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B524" s="6">
+        <v>43991</v>
+      </c>
+      <c r="C524" s="7">
+        <v>0.1035835012801727</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A525" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B525" s="6">
+        <v>43992</v>
+      </c>
+      <c r="C525" s="7">
+        <v>0.1067528849656571</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A526" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B526" s="6">
+        <v>43993</v>
+      </c>
+      <c r="C526" s="7">
+        <v>0.11009558994350724</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A527" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B527" s="6">
+        <v>43994</v>
+      </c>
+      <c r="C527" s="7">
+        <v>0.10696202665306526</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A528" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B528" s="6">
+        <v>43995</v>
+      </c>
+      <c r="C528" s="7">
+        <v>0.12623323428539993</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A529" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B529" s="6">
+        <v>43996</v>
+      </c>
+      <c r="C529" s="7">
+        <v>0.97377397612062566</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A530" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B530" s="6">
+        <v>43997</v>
+      </c>
+      <c r="C530" s="7">
+        <v>0.23859121969602365</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A531" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B531" s="6">
+        <v>43998</v>
+      </c>
+      <c r="C531" s="7">
+        <v>0.17592911691330651</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A532" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B532" s="6">
+        <v>43999</v>
+      </c>
+      <c r="C532" s="7">
+        <v>0.10590352956415552</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A533" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B533" s="6">
+        <v>44000</v>
+      </c>
+      <c r="C533" s="7">
+        <v>0.10143298682425388</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A534" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B534" s="6">
+        <v>44001</v>
+      </c>
+      <c r="C534" s="7">
+        <v>0.10421629506159467</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A535" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B535" s="6">
+        <v>44002</v>
+      </c>
+      <c r="C535" s="7">
+        <v>0.11152194049030742</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A536" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B536" s="6">
+        <v>44003</v>
+      </c>
+      <c r="C536" s="7">
+        <v>0.10144760300639108</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A537" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B537" s="6">
+        <v>44004</v>
+      </c>
+      <c r="C537" s="7">
+        <v>0.10573632623418319</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A538" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B538" s="6">
+        <v>44005</v>
+      </c>
+      <c r="C538" s="7">
+        <v>9.8401046197887324E-2</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A539" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B539" s="6">
+        <v>44006</v>
+      </c>
+      <c r="C539" s="7">
+        <v>9.6799703700480688E-2</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A540" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B540" s="6">
+        <v>44007</v>
+      </c>
+      <c r="C540" s="7">
+        <v>0.10142367908312672</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A541" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B541" s="6">
+        <v>44008</v>
+      </c>
+      <c r="C541" s="7">
+        <v>0.10105800744907109</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A542" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B542" s="6">
+        <v>44009</v>
+      </c>
+      <c r="C542" s="7">
+        <v>9.5838574088452144E-2</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A543" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B543" s="6">
+        <v>44010</v>
+      </c>
+      <c r="C543" s="7">
+        <v>9.4128635780373199E-2</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A544" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B544" s="6">
+        <v>44011</v>
+      </c>
+      <c r="C544" s="7">
+        <v>9.6861968668168749E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>